<commit_message>
Add data for home mortage arrears
</commit_message>
<xml_diff>
--- a/docs/housing_story_content/housing data story_part2.xlsx
+++ b/docs/housing_story_content/housing data story_part2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Part 2 charts summary" sheetId="32" r:id="rId1"/>
@@ -17,14 +17,12 @@
     <sheet name="(17) housing vacancy" sheetId="22" r:id="rId3"/>
     <sheet name="(12) serviced zoned land" sheetId="11" r:id="rId4"/>
     <sheet name="(8) mortgages arrears" sheetId="7" r:id="rId5"/>
-    <sheet name="(14) SH waiting list" sheetId="19" r:id="rId6"/>
-    <sheet name="(20) PPPs housing ests" sheetId="25" r:id="rId7"/>
-    <sheet name="(11) traveller accommodation" sheetId="10" r:id="rId8"/>
-    <sheet name="(9) BTL arrears" sheetId="8" r:id="rId9"/>
+    <sheet name="Sheet1" sheetId="33" r:id="rId6"/>
+    <sheet name="(14) SH waiting list" sheetId="19" r:id="rId7"/>
+    <sheet name="(20) PPPs housing ests" sheetId="25" r:id="rId8"/>
+    <sheet name="(11) traveller accommodation" sheetId="10" r:id="rId9"/>
+    <sheet name="(9) BTL arrears" sheetId="8" r:id="rId10"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId10"/>
-  </externalReferences>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -46,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="318">
   <si>
     <t>Fingal</t>
   </si>
@@ -1045,6 +1043,9 @@
   <si>
     <t>Tab 9 – Central Bank</t>
   </si>
+  <si>
+    <t>date</t>
+  </si>
 </sst>
 </file>
 
@@ -1053,11 +1054,11 @@
   <numFmts count="7">
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="169" formatCode="0000"/>
-    <numFmt numFmtId="170" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="171" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;?_-;_-@_-"/>
-    <numFmt numFmtId="172" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="0000"/>
+    <numFmt numFmtId="167" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="168" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;?_-;_-@_-"/>
+    <numFmt numFmtId="169" formatCode="0.0"/>
   </numFmts>
   <fonts count="22" x14ac:knownFonts="1">
     <font>
@@ -2514,9 +2515,9 @@
     <xf numFmtId="41" fontId="3" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="41" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="10" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="10" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="10" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="9" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2554,17 +2555,17 @@
     </xf>
     <xf numFmtId="17" fontId="4" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="41" fontId="3" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
@@ -2584,10 +2585,10 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="728"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="172" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="41" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3404,219 +3405,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="19 (2)"/>
-      <sheetName val="Index"/>
-      <sheetName val="1"/>
-      <sheetName val="2"/>
-      <sheetName val="3"/>
-      <sheetName val="4"/>
-      <sheetName val="5"/>
-      <sheetName val="6"/>
-      <sheetName val="7"/>
-      <sheetName val="8"/>
-      <sheetName val="9"/>
-      <sheetName val="10"/>
-      <sheetName val="11"/>
-      <sheetName val="12"/>
-      <sheetName val="13"/>
-      <sheetName val="14"/>
-      <sheetName val="15"/>
-      <sheetName val="16"/>
-      <sheetName val="17"/>
-      <sheetName val="18"/>
-      <sheetName val="19"/>
-      <sheetName val="20"/>
-      <sheetName val="21"/>
-      <sheetName val="22"/>
-      <sheetName val="23"/>
-      <sheetName val="24"/>
-      <sheetName val="Sheet1"/>
-      <sheetName val="Sheet2"/>
-      <sheetName val="Sheet3"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="6">
-          <cell r="A6">
-            <v>35431</v>
-          </cell>
-          <cell r="B6">
-            <v>858.56336268581867</v>
-          </cell>
-          <cell r="D6">
-            <v>4.7371626720691822</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7">
-            <v>35796</v>
-          </cell>
-          <cell r="B7">
-            <v>1110.0461765040432</v>
-          </cell>
-          <cell r="D7">
-            <v>5.4201473462111478</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8">
-            <v>36161</v>
-          </cell>
-          <cell r="B8">
-            <v>1596.0061186115754</v>
-          </cell>
-          <cell r="D8">
-            <v>6.7727821710654581</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9">
-            <v>36526</v>
-          </cell>
-          <cell r="B9">
-            <v>2132.0735813395172</v>
-          </cell>
-          <cell r="D9">
-            <v>7.8755673069574357</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10">
-            <v>36892</v>
-          </cell>
-          <cell r="B10">
-            <v>2402.6642801893595</v>
-          </cell>
-          <cell r="D10">
-            <v>8.6039902603020924</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11">
-            <v>37257</v>
-          </cell>
-          <cell r="B11">
-            <v>2395.7332671513655</v>
-          </cell>
-          <cell r="D11">
-            <v>8.1782387763752489</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12">
-            <v>37622</v>
-          </cell>
-          <cell r="B12">
-            <v>3750.9907616068208</v>
-          </cell>
-          <cell r="D12">
-            <v>11.68423749059845</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="A13">
-            <v>37987</v>
-          </cell>
-          <cell r="B13">
-            <v>4641.6681053143529</v>
-          </cell>
-          <cell r="D13">
-            <v>13.045355963335355</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="A14">
-            <v>38353</v>
-          </cell>
-          <cell r="B14">
-            <v>5949.4991125017459</v>
-          </cell>
-          <cell r="D14">
-            <v>15.156414919503097</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="A15">
-            <v>38718</v>
-          </cell>
-          <cell r="B15">
-            <v>8084.4846028054999</v>
-          </cell>
-          <cell r="D15">
-            <v>17.752881272767297</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="A16">
-            <v>39083.133333333302</v>
-          </cell>
-          <cell r="B16">
-            <v>6062.9820111814297</v>
-          </cell>
-          <cell r="D16">
-            <v>12.831979536458823</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="A17">
-            <v>39448.375757575799</v>
-          </cell>
-          <cell r="B17">
-            <v>2596.1946262460738</v>
-          </cell>
-          <cell r="D17">
-            <v>6.3669417904197019</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="A18" t="str">
-            <v>2009E</v>
-          </cell>
-          <cell r="B18">
-            <v>911.9982504984298</v>
-          </cell>
-          <cell r="D18">
-            <v>2.7600346533257567</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27"/>
-      <sheetData sheetId="28"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -4114,6 +3902,592 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C1:AN20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="65.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="28" width="9.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:29" x14ac:dyDescent="0.2">
+      <c r="C1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
+        <v>255</v>
+      </c>
+      <c r="G1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="2" spans="3:29" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="3:29" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="3:29" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="3:29" x14ac:dyDescent="0.2">
+      <c r="E7" s="20">
+        <v>41089</v>
+      </c>
+      <c r="F7" s="20">
+        <v>41180</v>
+      </c>
+      <c r="G7" s="20">
+        <v>41274</v>
+      </c>
+      <c r="H7" s="20">
+        <v>41361</v>
+      </c>
+      <c r="I7" s="20">
+        <v>41453</v>
+      </c>
+      <c r="J7" s="20">
+        <v>41547</v>
+      </c>
+      <c r="K7" s="20">
+        <v>41639</v>
+      </c>
+      <c r="L7" s="20">
+        <v>41729</v>
+      </c>
+      <c r="M7" s="20">
+        <v>41820</v>
+      </c>
+      <c r="N7" s="20">
+        <v>41912</v>
+      </c>
+      <c r="O7" s="20">
+        <v>42004</v>
+      </c>
+      <c r="P7" s="20">
+        <v>42094</v>
+      </c>
+      <c r="Q7" s="20">
+        <v>42185</v>
+      </c>
+      <c r="R7" s="20">
+        <v>42277</v>
+      </c>
+      <c r="S7" s="20">
+        <v>42369</v>
+      </c>
+      <c r="T7" s="20">
+        <v>42460</v>
+      </c>
+      <c r="U7" s="20">
+        <v>42551</v>
+      </c>
+      <c r="V7" s="20">
+        <v>42643</v>
+      </c>
+      <c r="W7" s="20">
+        <v>42734</v>
+      </c>
+      <c r="X7" s="20">
+        <v>42825</v>
+      </c>
+      <c r="Y7" s="20">
+        <v>42916</v>
+      </c>
+      <c r="Z7" s="20">
+        <v>43007</v>
+      </c>
+      <c r="AA7" s="20">
+        <v>43098</v>
+      </c>
+      <c r="AB7" s="20">
+        <v>43188</v>
+      </c>
+      <c r="AC7" s="56">
+        <v>43280</v>
+      </c>
+    </row>
+    <row r="8" spans="3:29" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J8" t="s">
+        <v>16</v>
+      </c>
+      <c r="K8" t="s">
+        <v>16</v>
+      </c>
+      <c r="L8" t="s">
+        <v>16</v>
+      </c>
+      <c r="M8" t="s">
+        <v>16</v>
+      </c>
+      <c r="N8" t="s">
+        <v>16</v>
+      </c>
+      <c r="O8" t="s">
+        <v>16</v>
+      </c>
+      <c r="P8" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>16</v>
+      </c>
+      <c r="R8" t="s">
+        <v>16</v>
+      </c>
+      <c r="S8" t="s">
+        <v>16</v>
+      </c>
+      <c r="T8" t="s">
+        <v>16</v>
+      </c>
+      <c r="U8" t="s">
+        <v>16</v>
+      </c>
+      <c r="V8" t="s">
+        <v>16</v>
+      </c>
+      <c r="W8" t="s">
+        <v>16</v>
+      </c>
+      <c r="X8" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="3:29" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="10" spans="3:29" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>224</v>
+      </c>
+      <c r="E10">
+        <v>150187</v>
+      </c>
+      <c r="F10">
+        <v>150544</v>
+      </c>
+      <c r="G10">
+        <v>150124</v>
+      </c>
+      <c r="H10">
+        <v>149395</v>
+      </c>
+      <c r="I10">
+        <v>148529</v>
+      </c>
+      <c r="J10">
+        <v>147610</v>
+      </c>
+      <c r="K10">
+        <v>145528</v>
+      </c>
+      <c r="L10">
+        <v>144686</v>
+      </c>
+      <c r="M10">
+        <v>144187</v>
+      </c>
+      <c r="N10">
+        <v>143354</v>
+      </c>
+      <c r="O10">
+        <v>140995</v>
+      </c>
+      <c r="P10">
+        <v>139206</v>
+      </c>
+      <c r="Q10">
+        <v>137303</v>
+      </c>
+      <c r="R10">
+        <v>137805</v>
+      </c>
+      <c r="S10">
+        <v>137504</v>
+      </c>
+      <c r="T10">
+        <v>137239</v>
+      </c>
+      <c r="U10">
+        <v>135874</v>
+      </c>
+      <c r="V10">
+        <v>133401</v>
+      </c>
+      <c r="W10">
+        <v>131501</v>
+      </c>
+      <c r="X10">
+        <v>128899</v>
+      </c>
+      <c r="Y10">
+        <v>127704</v>
+      </c>
+      <c r="Z10">
+        <v>125381</v>
+      </c>
+      <c r="AA10">
+        <v>123269</v>
+      </c>
+      <c r="AB10">
+        <v>121029</v>
+      </c>
+      <c r="AC10">
+        <v>118234</v>
+      </c>
+    </row>
+    <row r="11" spans="3:29" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>253</v>
+      </c>
+      <c r="E11">
+        <v>34719</v>
+      </c>
+      <c r="F11">
+        <v>36635</v>
+      </c>
+      <c r="G11">
+        <v>37878</v>
+      </c>
+      <c r="H11">
+        <v>39371</v>
+      </c>
+      <c r="I11">
+        <v>39948</v>
+      </c>
+      <c r="J11">
+        <v>40396</v>
+      </c>
+      <c r="K11">
+        <v>39250</v>
+      </c>
+      <c r="L11">
+        <v>39361</v>
+      </c>
+      <c r="M11">
+        <v>39669</v>
+      </c>
+      <c r="N11">
+        <v>38463</v>
+      </c>
+      <c r="O11">
+        <v>35583</v>
+      </c>
+      <c r="P11">
+        <v>33475</v>
+      </c>
+      <c r="Q11">
+        <v>31524</v>
+      </c>
+      <c r="R11">
+        <v>30212</v>
+      </c>
+      <c r="S11">
+        <v>28760</v>
+      </c>
+      <c r="T11">
+        <v>28716</v>
+      </c>
+      <c r="U11">
+        <v>27793</v>
+      </c>
+      <c r="V11">
+        <v>26737</v>
+      </c>
+      <c r="W11">
+        <v>25871</v>
+      </c>
+      <c r="X11">
+        <v>25175</v>
+      </c>
+      <c r="Y11">
+        <v>24450</v>
+      </c>
+      <c r="Z11">
+        <v>23779</v>
+      </c>
+      <c r="AA11">
+        <v>23282</v>
+      </c>
+      <c r="AB11">
+        <v>22545</v>
+      </c>
+      <c r="AC11" s="57">
+        <v>21317</v>
+      </c>
+    </row>
+    <row r="12" spans="3:29" x14ac:dyDescent="0.2">
+      <c r="C12">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12">
+        <v>24879</v>
+      </c>
+      <c r="F12">
+        <v>27018</v>
+      </c>
+      <c r="G12">
+        <v>28366</v>
+      </c>
+      <c r="H12">
+        <v>29369</v>
+      </c>
+      <c r="I12">
+        <v>30326</v>
+      </c>
+      <c r="J12">
+        <v>31178</v>
+      </c>
+      <c r="K12">
+        <v>30706</v>
+      </c>
+      <c r="L12">
+        <v>31048</v>
+      </c>
+      <c r="M12">
+        <v>31749</v>
+      </c>
+      <c r="N12">
+        <v>31619</v>
+      </c>
+      <c r="O12">
+        <v>29224</v>
+      </c>
+      <c r="P12">
+        <v>27492</v>
+      </c>
+      <c r="Q12">
+        <v>26071</v>
+      </c>
+      <c r="R12">
+        <v>24809</v>
+      </c>
+      <c r="S12">
+        <v>23344</v>
+      </c>
+      <c r="T12">
+        <v>23270</v>
+      </c>
+      <c r="U12">
+        <v>22666</v>
+      </c>
+      <c r="V12">
+        <v>22095</v>
+      </c>
+      <c r="W12">
+        <v>21113</v>
+      </c>
+      <c r="X12">
+        <v>20601</v>
+      </c>
+      <c r="Y12">
+        <v>20191</v>
+      </c>
+      <c r="Z12">
+        <v>19405</v>
+      </c>
+      <c r="AA12">
+        <v>19018</v>
+      </c>
+      <c r="AB12">
+        <v>18363</v>
+      </c>
+      <c r="AC12">
+        <v>17394</v>
+      </c>
+    </row>
+    <row r="13" spans="3:29" x14ac:dyDescent="0.2">
+      <c r="C13">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="F13">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="G13">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="H13">
+        <v>19.7</v>
+      </c>
+      <c r="I13">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="J13">
+        <v>21.1</v>
+      </c>
+      <c r="K13">
+        <v>21.1</v>
+      </c>
+      <c r="L13">
+        <v>21.5</v>
+      </c>
+      <c r="M13">
+        <v>22</v>
+      </c>
+      <c r="N13">
+        <v>22.1</v>
+      </c>
+      <c r="O13">
+        <v>20.7</v>
+      </c>
+      <c r="P13">
+        <v>19.7</v>
+      </c>
+      <c r="Q13">
+        <v>19</v>
+      </c>
+      <c r="R13">
+        <v>18</v>
+      </c>
+      <c r="S13">
+        <v>17</v>
+      </c>
+      <c r="T13">
+        <v>17</v>
+      </c>
+      <c r="U13">
+        <v>16.7</v>
+      </c>
+      <c r="V13">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="W13">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="X13">
+        <v>16</v>
+      </c>
+      <c r="Y13">
+        <v>15.8</v>
+      </c>
+      <c r="Z13">
+        <v>15.5</v>
+      </c>
+      <c r="AA13">
+        <v>15.4</v>
+      </c>
+      <c r="AB13">
+        <v>15.2</v>
+      </c>
+      <c r="AC13">
+        <v>14.7</v>
+      </c>
+    </row>
+    <row r="20" spans="4:40" x14ac:dyDescent="0.2">
+      <c r="D20" s="21"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="22"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="22"/>
+      <c r="N20" s="23"/>
+      <c r="O20" s="22"/>
+      <c r="P20" s="23"/>
+      <c r="Q20" s="22"/>
+      <c r="R20" s="23"/>
+      <c r="S20" s="22"/>
+      <c r="T20" s="23"/>
+      <c r="U20" s="22"/>
+      <c r="V20" s="23"/>
+      <c r="W20" s="22"/>
+      <c r="X20" s="23"/>
+      <c r="Y20" s="22"/>
+      <c r="Z20" s="23"/>
+      <c r="AA20" s="22"/>
+      <c r="AB20" s="23"/>
+      <c r="AC20" s="22"/>
+      <c r="AD20" s="23"/>
+      <c r="AE20" s="22"/>
+      <c r="AF20" s="23"/>
+      <c r="AG20" s="22"/>
+      <c r="AH20" s="23"/>
+      <c r="AI20" s="22"/>
+      <c r="AJ20" s="23"/>
+      <c r="AK20" s="22"/>
+      <c r="AL20" s="23"/>
+      <c r="AM20" s="22"/>
+      <c r="AN20" s="27"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H168"/>
@@ -7949,7 +8323,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
@@ -9980,15 +10354,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:AM18"/>
+  <dimension ref="A1:AM57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10:G13"/>
+    <sheetView topLeftCell="A29" zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.33203125" customWidth="1"/>
     <col min="3" max="3" width="55.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="39" width="9.6640625" bestFit="1" customWidth="1"/>
@@ -10872,7 +11246,7 @@
       <c r="AL16" s="25"/>
       <c r="AM16" s="28"/>
     </row>
-    <row r="17" spans="3:39" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.2">
       <c r="C17" s="21"/>
       <c r="D17" s="22"/>
       <c r="E17" s="23"/>
@@ -10911,7 +11285,7 @@
       <c r="AL17" s="22"/>
       <c r="AM17" s="27"/>
     </row>
-    <row r="18" spans="3:39" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:39" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C18" s="29"/>
       <c r="D18" s="30"/>
       <c r="E18" s="31"/>
@@ -10950,6 +11324,632 @@
       <c r="AL18" s="30"/>
       <c r="AM18" s="32"/>
     </row>
+    <row r="21" spans="1:39" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>253</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:39" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="11">
+        <v>40086</v>
+      </c>
+      <c r="B22" s="10">
+        <v>794609</v>
+      </c>
+      <c r="C22" s="10">
+        <v>63619</v>
+      </c>
+      <c r="D22" s="60">
+        <v>26271</v>
+      </c>
+      <c r="E22" s="58">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:39" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="11">
+        <v>40178</v>
+      </c>
+      <c r="B23" s="10">
+        <v>792885</v>
+      </c>
+      <c r="C23" s="10">
+        <v>69647</v>
+      </c>
+      <c r="D23" s="60">
+        <v>28603</v>
+      </c>
+      <c r="E23" s="58">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:39" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="11">
+        <v>40268</v>
+      </c>
+      <c r="B24" s="10">
+        <v>791047</v>
+      </c>
+      <c r="C24" s="10">
+        <v>76100</v>
+      </c>
+      <c r="D24" s="60">
+        <v>32321</v>
+      </c>
+      <c r="E24" s="58">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="25" spans="1:39" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="11">
+        <v>40359</v>
+      </c>
+      <c r="B25" s="10">
+        <v>789814</v>
+      </c>
+      <c r="C25" s="10">
+        <v>82377</v>
+      </c>
+      <c r="D25" s="60">
+        <v>36438</v>
+      </c>
+      <c r="E25" s="58">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="26" spans="1:39" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="11">
+        <v>40451</v>
+      </c>
+      <c r="B26" s="10">
+        <v>788745</v>
+      </c>
+      <c r="C26" s="10">
+        <v>86362</v>
+      </c>
+      <c r="D26" s="60">
+        <v>40472</v>
+      </c>
+      <c r="E26" s="58">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="27" spans="1:39" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="11">
+        <v>40543</v>
+      </c>
+      <c r="B27" s="10">
+        <v>786164</v>
+      </c>
+      <c r="C27" s="10">
+        <v>89234</v>
+      </c>
+      <c r="D27" s="60">
+        <v>44508</v>
+      </c>
+      <c r="E27" s="58">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:39" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="11">
+        <v>40633</v>
+      </c>
+      <c r="B28" s="10">
+        <v>782429</v>
+      </c>
+      <c r="C28" s="10">
+        <v>94518</v>
+      </c>
+      <c r="D28" s="60">
+        <v>49609</v>
+      </c>
+      <c r="E28" s="58">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:39" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="11">
+        <v>40724</v>
+      </c>
+      <c r="B29" s="10">
+        <v>777321</v>
+      </c>
+      <c r="C29" s="10">
+        <v>102397</v>
+      </c>
+      <c r="D29" s="60">
+        <v>55763</v>
+      </c>
+      <c r="E29" s="58">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:39" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="11">
+        <v>40816</v>
+      </c>
+      <c r="B30" s="10">
+        <v>773420</v>
+      </c>
+      <c r="C30" s="10">
+        <v>110597</v>
+      </c>
+      <c r="D30" s="60">
+        <v>62970</v>
+      </c>
+      <c r="E30" s="58">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:39" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="11">
+        <v>40907</v>
+      </c>
+      <c r="B31" s="10">
+        <v>768955</v>
+      </c>
+      <c r="C31" s="10">
+        <v>118464</v>
+      </c>
+      <c r="D31" s="60">
+        <v>69354</v>
+      </c>
+      <c r="E31" s="58">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:39" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="11">
+        <v>40998</v>
+      </c>
+      <c r="B32" s="10">
+        <v>764138</v>
+      </c>
+      <c r="C32" s="10">
+        <v>122941</v>
+      </c>
+      <c r="D32" s="60">
+        <v>75679</v>
+      </c>
+      <c r="E32" s="58">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="11">
+        <v>41089</v>
+      </c>
+      <c r="B33" s="10">
+        <v>765267</v>
+      </c>
+      <c r="C33" s="10">
+        <v>128197</v>
+      </c>
+      <c r="D33" s="60">
+        <v>81035</v>
+      </c>
+      <c r="E33" s="58">
+        <v>10.6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="11">
+        <v>41180</v>
+      </c>
+      <c r="B34" s="10">
+        <v>794275</v>
+      </c>
+      <c r="C34" s="10">
+        <v>141389</v>
+      </c>
+      <c r="D34" s="60">
+        <v>91358</v>
+      </c>
+      <c r="E34" s="58">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="11">
+        <v>41274</v>
+      </c>
+      <c r="B35" s="10">
+        <v>778375</v>
+      </c>
+      <c r="C35" s="10">
+        <v>139224</v>
+      </c>
+      <c r="D35" s="60">
+        <v>92349</v>
+      </c>
+      <c r="E35" s="58">
+        <v>11.9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="11">
+        <v>41361</v>
+      </c>
+      <c r="B36" s="10">
+        <v>774109</v>
+      </c>
+      <c r="C36" s="10">
+        <v>142118</v>
+      </c>
+      <c r="D36" s="60">
+        <v>95554</v>
+      </c>
+      <c r="E36" s="58">
+        <v>12.3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="11">
+        <v>41453</v>
+      </c>
+      <c r="B37" s="10">
+        <v>770610</v>
+      </c>
+      <c r="C37" s="10">
+        <v>142892</v>
+      </c>
+      <c r="D37" s="60">
+        <v>97874</v>
+      </c>
+      <c r="E37" s="58">
+        <v>12.7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="11">
+        <v>41547</v>
+      </c>
+      <c r="B38" s="10">
+        <v>768136</v>
+      </c>
+      <c r="C38" s="10">
+        <v>141269</v>
+      </c>
+      <c r="D38" s="60">
+        <v>98736</v>
+      </c>
+      <c r="E38" s="58">
+        <v>12.9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="11">
+        <v>41639</v>
+      </c>
+      <c r="B39" s="10">
+        <v>764541</v>
+      </c>
+      <c r="C39" s="10">
+        <v>136558</v>
+      </c>
+      <c r="D39" s="60">
+        <v>96467</v>
+      </c>
+      <c r="E39" s="58">
+        <v>12.6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="11">
+        <v>41729</v>
+      </c>
+      <c r="B40" s="10">
+        <v>762454</v>
+      </c>
+      <c r="C40" s="10">
+        <v>132217</v>
+      </c>
+      <c r="D40" s="60">
+        <v>93106</v>
+      </c>
+      <c r="E40" s="58">
+        <v>12.2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="11">
+        <v>41820</v>
+      </c>
+      <c r="B41" s="10">
+        <v>762575</v>
+      </c>
+      <c r="C41" s="10">
+        <v>126005</v>
+      </c>
+      <c r="D41" s="60">
+        <v>90343</v>
+      </c>
+      <c r="E41" s="58">
+        <v>11.8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="11">
+        <v>41912</v>
+      </c>
+      <c r="B42" s="10">
+        <v>760238</v>
+      </c>
+      <c r="C42" s="10">
+        <v>117889</v>
+      </c>
+      <c r="D42" s="60">
+        <v>84955</v>
+      </c>
+      <c r="E42" s="58">
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="11">
+        <v>42004</v>
+      </c>
+      <c r="B43" s="10">
+        <v>758988</v>
+      </c>
+      <c r="C43" s="10">
+        <v>110366</v>
+      </c>
+      <c r="D43" s="60">
+        <v>78699</v>
+      </c>
+      <c r="E43" s="58">
+        <v>10.4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="11">
+        <v>42094</v>
+      </c>
+      <c r="B44" s="10">
+        <v>757175</v>
+      </c>
+      <c r="C44" s="10">
+        <v>104693</v>
+      </c>
+      <c r="D44" s="60">
+        <v>74395</v>
+      </c>
+      <c r="E44" s="58">
+        <v>9.8000000000000007</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="11">
+        <v>42185</v>
+      </c>
+      <c r="B45" s="10">
+        <v>754688</v>
+      </c>
+      <c r="C45" s="10">
+        <v>98155</v>
+      </c>
+      <c r="D45" s="60">
+        <v>70296</v>
+      </c>
+      <c r="E45" s="58">
+        <v>9.3000000000000007</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="11">
+        <v>42277</v>
+      </c>
+      <c r="B46" s="10">
+        <v>749851</v>
+      </c>
+      <c r="C46" s="10">
+        <v>92361</v>
+      </c>
+      <c r="D46" s="60">
+        <v>65653</v>
+      </c>
+      <c r="E46" s="59">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="11">
+        <v>42369</v>
+      </c>
+      <c r="B47" s="10">
+        <v>746618</v>
+      </c>
+      <c r="C47" s="10">
+        <v>88292</v>
+      </c>
+      <c r="D47" s="60">
+        <v>61931</v>
+      </c>
+      <c r="E47">
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="11">
+        <v>42460</v>
+      </c>
+      <c r="B48" s="10">
+        <v>744685</v>
+      </c>
+      <c r="C48" s="10">
+        <v>86808</v>
+      </c>
+      <c r="D48" s="60">
+        <v>60453</v>
+      </c>
+      <c r="E48">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="11">
+        <v>42551</v>
+      </c>
+      <c r="B49" s="10">
+        <v>741785</v>
+      </c>
+      <c r="C49" s="10">
+        <v>82882</v>
+      </c>
+      <c r="D49" s="60">
+        <v>58309</v>
+      </c>
+      <c r="E49">
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="11">
+        <v>42643</v>
+      </c>
+      <c r="B50" s="10">
+        <v>739421</v>
+      </c>
+      <c r="C50" s="10">
+        <v>80321</v>
+      </c>
+      <c r="D50" s="60">
+        <v>57067</v>
+      </c>
+      <c r="E50">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="11">
+        <v>42734</v>
+      </c>
+      <c r="B51" s="10">
+        <v>737795</v>
+      </c>
+      <c r="C51" s="10">
+        <v>78249</v>
+      </c>
+      <c r="D51" s="60">
+        <v>54977</v>
+      </c>
+      <c r="E51">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="11">
+        <v>42825</v>
+      </c>
+      <c r="B52" s="10">
+        <v>734976</v>
+      </c>
+      <c r="C52" s="10">
+        <v>77146</v>
+      </c>
+      <c r="D52" s="60">
+        <v>53793</v>
+      </c>
+      <c r="E52">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="11">
+        <v>42916</v>
+      </c>
+      <c r="B53" s="10">
+        <v>733289</v>
+      </c>
+      <c r="C53" s="10">
+        <v>74410</v>
+      </c>
+      <c r="D53" s="60">
+        <v>52419</v>
+      </c>
+      <c r="E53">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="11">
+        <v>43007</v>
+      </c>
+      <c r="B54" s="10">
+        <v>731928</v>
+      </c>
+      <c r="C54" s="10">
+        <v>73197</v>
+      </c>
+      <c r="D54" s="60">
+        <v>51327</v>
+      </c>
+      <c r="E54">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="11">
+        <v>43098</v>
+      </c>
+      <c r="B55" s="10">
+        <v>730856</v>
+      </c>
+      <c r="C55" s="10">
+        <v>71517</v>
+      </c>
+      <c r="D55" s="60">
+        <v>49386</v>
+      </c>
+      <c r="E55">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="11">
+        <v>43188</v>
+      </c>
+      <c r="B56" s="10">
+        <v>728575</v>
+      </c>
+      <c r="C56" s="10">
+        <v>71833</v>
+      </c>
+      <c r="D56" s="60">
+        <v>48538</v>
+      </c>
+      <c r="E56">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="12">
+        <v>43280</v>
+      </c>
+      <c r="B57" s="13">
+        <v>725693</v>
+      </c>
+      <c r="C57" s="13">
+        <v>66479</v>
+      </c>
+      <c r="D57" s="61">
+        <v>46008</v>
+      </c>
+      <c r="E57">
+        <v>6.3</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1"/>
@@ -10959,6 +11959,650 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>317</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>253</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11">
+        <v>40086</v>
+      </c>
+      <c r="B2" s="10">
+        <v>794609</v>
+      </c>
+      <c r="C2" s="10">
+        <v>63619</v>
+      </c>
+      <c r="D2" s="60">
+        <v>26271</v>
+      </c>
+      <c r="E2" s="58">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11">
+        <v>40178</v>
+      </c>
+      <c r="B3" s="10">
+        <v>792885</v>
+      </c>
+      <c r="C3" s="10">
+        <v>69647</v>
+      </c>
+      <c r="D3" s="60">
+        <v>28603</v>
+      </c>
+      <c r="E3" s="58">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
+        <v>40268</v>
+      </c>
+      <c r="B4" s="10">
+        <v>791047</v>
+      </c>
+      <c r="C4" s="10">
+        <v>76100</v>
+      </c>
+      <c r="D4" s="60">
+        <v>32321</v>
+      </c>
+      <c r="E4" s="58">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="11">
+        <v>40359</v>
+      </c>
+      <c r="B5" s="10">
+        <v>789814</v>
+      </c>
+      <c r="C5" s="10">
+        <v>82377</v>
+      </c>
+      <c r="D5" s="60">
+        <v>36438</v>
+      </c>
+      <c r="E5" s="58">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="11">
+        <v>40451</v>
+      </c>
+      <c r="B6" s="10">
+        <v>788745</v>
+      </c>
+      <c r="C6" s="10">
+        <v>86362</v>
+      </c>
+      <c r="D6" s="60">
+        <v>40472</v>
+      </c>
+      <c r="E6" s="58">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
+        <v>40543</v>
+      </c>
+      <c r="B7" s="10">
+        <v>786164</v>
+      </c>
+      <c r="C7" s="10">
+        <v>89234</v>
+      </c>
+      <c r="D7" s="60">
+        <v>44508</v>
+      </c>
+      <c r="E7" s="58">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11">
+        <v>40633</v>
+      </c>
+      <c r="B8" s="10">
+        <v>782429</v>
+      </c>
+      <c r="C8" s="10">
+        <v>94518</v>
+      </c>
+      <c r="D8" s="60">
+        <v>49609</v>
+      </c>
+      <c r="E8" s="58">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11">
+        <v>40724</v>
+      </c>
+      <c r="B9" s="10">
+        <v>777321</v>
+      </c>
+      <c r="C9" s="10">
+        <v>102397</v>
+      </c>
+      <c r="D9" s="60">
+        <v>55763</v>
+      </c>
+      <c r="E9" s="58">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="11">
+        <v>40816</v>
+      </c>
+      <c r="B10" s="10">
+        <v>773420</v>
+      </c>
+      <c r="C10" s="10">
+        <v>110597</v>
+      </c>
+      <c r="D10" s="60">
+        <v>62970</v>
+      </c>
+      <c r="E10" s="58">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="11">
+        <v>40907</v>
+      </c>
+      <c r="B11" s="10">
+        <v>768955</v>
+      </c>
+      <c r="C11" s="10">
+        <v>118464</v>
+      </c>
+      <c r="D11" s="60">
+        <v>69354</v>
+      </c>
+      <c r="E11" s="58">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="11">
+        <v>40998</v>
+      </c>
+      <c r="B12" s="10">
+        <v>764138</v>
+      </c>
+      <c r="C12" s="10">
+        <v>122941</v>
+      </c>
+      <c r="D12" s="60">
+        <v>75679</v>
+      </c>
+      <c r="E12" s="58">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="11">
+        <v>41089</v>
+      </c>
+      <c r="B13" s="10">
+        <v>765267</v>
+      </c>
+      <c r="C13" s="10">
+        <v>128197</v>
+      </c>
+      <c r="D13" s="60">
+        <v>81035</v>
+      </c>
+      <c r="E13" s="58">
+        <v>10.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="11">
+        <v>41180</v>
+      </c>
+      <c r="B14" s="10">
+        <v>794275</v>
+      </c>
+      <c r="C14" s="10">
+        <v>141389</v>
+      </c>
+      <c r="D14" s="60">
+        <v>91358</v>
+      </c>
+      <c r="E14" s="58">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="11">
+        <v>41274</v>
+      </c>
+      <c r="B15" s="10">
+        <v>778375</v>
+      </c>
+      <c r="C15" s="10">
+        <v>139224</v>
+      </c>
+      <c r="D15" s="60">
+        <v>92349</v>
+      </c>
+      <c r="E15" s="58">
+        <v>11.9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="11">
+        <v>41361</v>
+      </c>
+      <c r="B16" s="10">
+        <v>774109</v>
+      </c>
+      <c r="C16" s="10">
+        <v>142118</v>
+      </c>
+      <c r="D16" s="60">
+        <v>95554</v>
+      </c>
+      <c r="E16" s="58">
+        <v>12.3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="11">
+        <v>41453</v>
+      </c>
+      <c r="B17" s="10">
+        <v>770610</v>
+      </c>
+      <c r="C17" s="10">
+        <v>142892</v>
+      </c>
+      <c r="D17" s="60">
+        <v>97874</v>
+      </c>
+      <c r="E17" s="58">
+        <v>12.7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="11">
+        <v>41547</v>
+      </c>
+      <c r="B18" s="10">
+        <v>768136</v>
+      </c>
+      <c r="C18" s="10">
+        <v>141269</v>
+      </c>
+      <c r="D18" s="60">
+        <v>98736</v>
+      </c>
+      <c r="E18" s="58">
+        <v>12.9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="11">
+        <v>41639</v>
+      </c>
+      <c r="B19" s="10">
+        <v>764541</v>
+      </c>
+      <c r="C19" s="10">
+        <v>136558</v>
+      </c>
+      <c r="D19" s="60">
+        <v>96467</v>
+      </c>
+      <c r="E19" s="58">
+        <v>12.6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="11">
+        <v>41729</v>
+      </c>
+      <c r="B20" s="10">
+        <v>762454</v>
+      </c>
+      <c r="C20" s="10">
+        <v>132217</v>
+      </c>
+      <c r="D20" s="60">
+        <v>93106</v>
+      </c>
+      <c r="E20" s="58">
+        <v>12.2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="11">
+        <v>41820</v>
+      </c>
+      <c r="B21" s="10">
+        <v>762575</v>
+      </c>
+      <c r="C21" s="10">
+        <v>126005</v>
+      </c>
+      <c r="D21" s="60">
+        <v>90343</v>
+      </c>
+      <c r="E21" s="58">
+        <v>11.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="11">
+        <v>41912</v>
+      </c>
+      <c r="B22" s="10">
+        <v>760238</v>
+      </c>
+      <c r="C22" s="10">
+        <v>117889</v>
+      </c>
+      <c r="D22" s="60">
+        <v>84955</v>
+      </c>
+      <c r="E22" s="58">
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="11">
+        <v>42004</v>
+      </c>
+      <c r="B23" s="10">
+        <v>758988</v>
+      </c>
+      <c r="C23" s="10">
+        <v>110366</v>
+      </c>
+      <c r="D23" s="60">
+        <v>78699</v>
+      </c>
+      <c r="E23" s="58">
+        <v>10.4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="11">
+        <v>42094</v>
+      </c>
+      <c r="B24" s="10">
+        <v>757175</v>
+      </c>
+      <c r="C24" s="10">
+        <v>104693</v>
+      </c>
+      <c r="D24" s="60">
+        <v>74395</v>
+      </c>
+      <c r="E24" s="58">
+        <v>9.8000000000000007</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="11">
+        <v>42185</v>
+      </c>
+      <c r="B25" s="10">
+        <v>754688</v>
+      </c>
+      <c r="C25" s="10">
+        <v>98155</v>
+      </c>
+      <c r="D25" s="60">
+        <v>70296</v>
+      </c>
+      <c r="E25" s="58">
+        <v>9.3000000000000007</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="11">
+        <v>42277</v>
+      </c>
+      <c r="B26" s="10">
+        <v>749851</v>
+      </c>
+      <c r="C26" s="10">
+        <v>92361</v>
+      </c>
+      <c r="D26" s="60">
+        <v>65653</v>
+      </c>
+      <c r="E26" s="59">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="11">
+        <v>42369</v>
+      </c>
+      <c r="B27" s="10">
+        <v>746618</v>
+      </c>
+      <c r="C27" s="10">
+        <v>88292</v>
+      </c>
+      <c r="D27" s="60">
+        <v>61931</v>
+      </c>
+      <c r="E27">
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="11">
+        <v>42460</v>
+      </c>
+      <c r="B28" s="10">
+        <v>744685</v>
+      </c>
+      <c r="C28" s="10">
+        <v>86808</v>
+      </c>
+      <c r="D28" s="60">
+        <v>60453</v>
+      </c>
+      <c r="E28">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="11">
+        <v>42551</v>
+      </c>
+      <c r="B29" s="10">
+        <v>741785</v>
+      </c>
+      <c r="C29" s="10">
+        <v>82882</v>
+      </c>
+      <c r="D29" s="60">
+        <v>58309</v>
+      </c>
+      <c r="E29">
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="11">
+        <v>42643</v>
+      </c>
+      <c r="B30" s="10">
+        <v>739421</v>
+      </c>
+      <c r="C30" s="10">
+        <v>80321</v>
+      </c>
+      <c r="D30" s="60">
+        <v>57067</v>
+      </c>
+      <c r="E30">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="11">
+        <v>42734</v>
+      </c>
+      <c r="B31" s="10">
+        <v>737795</v>
+      </c>
+      <c r="C31" s="10">
+        <v>78249</v>
+      </c>
+      <c r="D31" s="60">
+        <v>54977</v>
+      </c>
+      <c r="E31">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="11">
+        <v>42825</v>
+      </c>
+      <c r="B32" s="10">
+        <v>734976</v>
+      </c>
+      <c r="C32" s="10">
+        <v>77146</v>
+      </c>
+      <c r="D32" s="60">
+        <v>53793</v>
+      </c>
+      <c r="E32">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="11">
+        <v>42916</v>
+      </c>
+      <c r="B33" s="10">
+        <v>733289</v>
+      </c>
+      <c r="C33" s="10">
+        <v>74410</v>
+      </c>
+      <c r="D33" s="60">
+        <v>52419</v>
+      </c>
+      <c r="E33">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="11">
+        <v>43007</v>
+      </c>
+      <c r="B34" s="10">
+        <v>731928</v>
+      </c>
+      <c r="C34" s="10">
+        <v>73197</v>
+      </c>
+      <c r="D34" s="60">
+        <v>51327</v>
+      </c>
+      <c r="E34">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="11">
+        <v>43098</v>
+      </c>
+      <c r="B35" s="10">
+        <v>730856</v>
+      </c>
+      <c r="C35" s="10">
+        <v>71517</v>
+      </c>
+      <c r="D35" s="60">
+        <v>49386</v>
+      </c>
+      <c r="E35">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="11">
+        <v>43188</v>
+      </c>
+      <c r="B36" s="10">
+        <v>728575</v>
+      </c>
+      <c r="C36" s="10">
+        <v>71833</v>
+      </c>
+      <c r="D36" s="60">
+        <v>48538</v>
+      </c>
+      <c r="E36">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="12">
+        <v>43280</v>
+      </c>
+      <c r="B37" s="13">
+        <v>725693</v>
+      </c>
+      <c r="C37" s="13">
+        <v>66479</v>
+      </c>
+      <c r="D37" s="61">
+        <v>46008</v>
+      </c>
+      <c r="E37">
+        <v>6.3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:P22"/>
   <sheetViews>
@@ -11274,7 +12918,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E13"/>
   <sheetViews>
@@ -11432,7 +13076,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:BV24"/>
   <sheetViews>
@@ -12668,592 +14312,6 @@
     <mergeCell ref="C4:N4"/>
     <mergeCell ref="O4:Z4"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:AN20"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="65.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="28" width="9.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="3:29" x14ac:dyDescent="0.2">
-      <c r="C1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" t="s">
-        <v>255</v>
-      </c>
-      <c r="G1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="2" spans="3:29" x14ac:dyDescent="0.2">
-      <c r="C2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="3:29" x14ac:dyDescent="0.2">
-      <c r="C3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="3:29" x14ac:dyDescent="0.2">
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="3:29" x14ac:dyDescent="0.2">
-      <c r="E7" s="20">
-        <v>41089</v>
-      </c>
-      <c r="F7" s="20">
-        <v>41180</v>
-      </c>
-      <c r="G7" s="20">
-        <v>41274</v>
-      </c>
-      <c r="H7" s="20">
-        <v>41361</v>
-      </c>
-      <c r="I7" s="20">
-        <v>41453</v>
-      </c>
-      <c r="J7" s="20">
-        <v>41547</v>
-      </c>
-      <c r="K7" s="20">
-        <v>41639</v>
-      </c>
-      <c r="L7" s="20">
-        <v>41729</v>
-      </c>
-      <c r="M7" s="20">
-        <v>41820</v>
-      </c>
-      <c r="N7" s="20">
-        <v>41912</v>
-      </c>
-      <c r="O7" s="20">
-        <v>42004</v>
-      </c>
-      <c r="P7" s="20">
-        <v>42094</v>
-      </c>
-      <c r="Q7" s="20">
-        <v>42185</v>
-      </c>
-      <c r="R7" s="20">
-        <v>42277</v>
-      </c>
-      <c r="S7" s="20">
-        <v>42369</v>
-      </c>
-      <c r="T7" s="20">
-        <v>42460</v>
-      </c>
-      <c r="U7" s="20">
-        <v>42551</v>
-      </c>
-      <c r="V7" s="20">
-        <v>42643</v>
-      </c>
-      <c r="W7" s="20">
-        <v>42734</v>
-      </c>
-      <c r="X7" s="20">
-        <v>42825</v>
-      </c>
-      <c r="Y7" s="20">
-        <v>42916</v>
-      </c>
-      <c r="Z7" s="20">
-        <v>43007</v>
-      </c>
-      <c r="AA7" s="20">
-        <v>43098</v>
-      </c>
-      <c r="AB7" s="20">
-        <v>43188</v>
-      </c>
-      <c r="AC7" s="56">
-        <v>43280</v>
-      </c>
-    </row>
-    <row r="8" spans="3:29" x14ac:dyDescent="0.2">
-      <c r="C8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" t="s">
-        <v>16</v>
-      </c>
-      <c r="I8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J8" t="s">
-        <v>16</v>
-      </c>
-      <c r="K8" t="s">
-        <v>16</v>
-      </c>
-      <c r="L8" t="s">
-        <v>16</v>
-      </c>
-      <c r="M8" t="s">
-        <v>16</v>
-      </c>
-      <c r="N8" t="s">
-        <v>16</v>
-      </c>
-      <c r="O8" t="s">
-        <v>16</v>
-      </c>
-      <c r="P8" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>16</v>
-      </c>
-      <c r="R8" t="s">
-        <v>16</v>
-      </c>
-      <c r="S8" t="s">
-        <v>16</v>
-      </c>
-      <c r="T8" t="s">
-        <v>16</v>
-      </c>
-      <c r="U8" t="s">
-        <v>16</v>
-      </c>
-      <c r="V8" t="s">
-        <v>16</v>
-      </c>
-      <c r="W8" t="s">
-        <v>16</v>
-      </c>
-      <c r="X8" t="s">
-        <v>16</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>16</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>16</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>16</v>
-      </c>
-      <c r="AC8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="3:29" x14ac:dyDescent="0.2">
-      <c r="C9" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="10" spans="3:29" x14ac:dyDescent="0.2">
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>224</v>
-      </c>
-      <c r="E10">
-        <v>150187</v>
-      </c>
-      <c r="F10">
-        <v>150544</v>
-      </c>
-      <c r="G10">
-        <v>150124</v>
-      </c>
-      <c r="H10">
-        <v>149395</v>
-      </c>
-      <c r="I10">
-        <v>148529</v>
-      </c>
-      <c r="J10">
-        <v>147610</v>
-      </c>
-      <c r="K10">
-        <v>145528</v>
-      </c>
-      <c r="L10">
-        <v>144686</v>
-      </c>
-      <c r="M10">
-        <v>144187</v>
-      </c>
-      <c r="N10">
-        <v>143354</v>
-      </c>
-      <c r="O10">
-        <v>140995</v>
-      </c>
-      <c r="P10">
-        <v>139206</v>
-      </c>
-      <c r="Q10">
-        <v>137303</v>
-      </c>
-      <c r="R10">
-        <v>137805</v>
-      </c>
-      <c r="S10">
-        <v>137504</v>
-      </c>
-      <c r="T10">
-        <v>137239</v>
-      </c>
-      <c r="U10">
-        <v>135874</v>
-      </c>
-      <c r="V10">
-        <v>133401</v>
-      </c>
-      <c r="W10">
-        <v>131501</v>
-      </c>
-      <c r="X10">
-        <v>128899</v>
-      </c>
-      <c r="Y10">
-        <v>127704</v>
-      </c>
-      <c r="Z10">
-        <v>125381</v>
-      </c>
-      <c r="AA10">
-        <v>123269</v>
-      </c>
-      <c r="AB10">
-        <v>121029</v>
-      </c>
-      <c r="AC10">
-        <v>118234</v>
-      </c>
-    </row>
-    <row r="11" spans="3:29" x14ac:dyDescent="0.2">
-      <c r="C11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" t="s">
-        <v>253</v>
-      </c>
-      <c r="E11">
-        <v>34719</v>
-      </c>
-      <c r="F11">
-        <v>36635</v>
-      </c>
-      <c r="G11">
-        <v>37878</v>
-      </c>
-      <c r="H11">
-        <v>39371</v>
-      </c>
-      <c r="I11">
-        <v>39948</v>
-      </c>
-      <c r="J11">
-        <v>40396</v>
-      </c>
-      <c r="K11">
-        <v>39250</v>
-      </c>
-      <c r="L11">
-        <v>39361</v>
-      </c>
-      <c r="M11">
-        <v>39669</v>
-      </c>
-      <c r="N11">
-        <v>38463</v>
-      </c>
-      <c r="O11">
-        <v>35583</v>
-      </c>
-      <c r="P11">
-        <v>33475</v>
-      </c>
-      <c r="Q11">
-        <v>31524</v>
-      </c>
-      <c r="R11">
-        <v>30212</v>
-      </c>
-      <c r="S11">
-        <v>28760</v>
-      </c>
-      <c r="T11">
-        <v>28716</v>
-      </c>
-      <c r="U11">
-        <v>27793</v>
-      </c>
-      <c r="V11">
-        <v>26737</v>
-      </c>
-      <c r="W11">
-        <v>25871</v>
-      </c>
-      <c r="X11">
-        <v>25175</v>
-      </c>
-      <c r="Y11">
-        <v>24450</v>
-      </c>
-      <c r="Z11">
-        <v>23779</v>
-      </c>
-      <c r="AA11">
-        <v>23282</v>
-      </c>
-      <c r="AB11">
-        <v>22545</v>
-      </c>
-      <c r="AC11" s="57">
-        <v>21317</v>
-      </c>
-    </row>
-    <row r="12" spans="3:29" x14ac:dyDescent="0.2">
-      <c r="C12">
-        <v>9</v>
-      </c>
-      <c r="D12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12">
-        <v>24879</v>
-      </c>
-      <c r="F12">
-        <v>27018</v>
-      </c>
-      <c r="G12">
-        <v>28366</v>
-      </c>
-      <c r="H12">
-        <v>29369</v>
-      </c>
-      <c r="I12">
-        <v>30326</v>
-      </c>
-      <c r="J12">
-        <v>31178</v>
-      </c>
-      <c r="K12">
-        <v>30706</v>
-      </c>
-      <c r="L12">
-        <v>31048</v>
-      </c>
-      <c r="M12">
-        <v>31749</v>
-      </c>
-      <c r="N12">
-        <v>31619</v>
-      </c>
-      <c r="O12">
-        <v>29224</v>
-      </c>
-      <c r="P12">
-        <v>27492</v>
-      </c>
-      <c r="Q12">
-        <v>26071</v>
-      </c>
-      <c r="R12">
-        <v>24809</v>
-      </c>
-      <c r="S12">
-        <v>23344</v>
-      </c>
-      <c r="T12">
-        <v>23270</v>
-      </c>
-      <c r="U12">
-        <v>22666</v>
-      </c>
-      <c r="V12">
-        <v>22095</v>
-      </c>
-      <c r="W12">
-        <v>21113</v>
-      </c>
-      <c r="X12">
-        <v>20601</v>
-      </c>
-      <c r="Y12">
-        <v>20191</v>
-      </c>
-      <c r="Z12">
-        <v>19405</v>
-      </c>
-      <c r="AA12">
-        <v>19018</v>
-      </c>
-      <c r="AB12">
-        <v>18363</v>
-      </c>
-      <c r="AC12">
-        <v>17394</v>
-      </c>
-    </row>
-    <row r="13" spans="3:29" x14ac:dyDescent="0.2">
-      <c r="C13">
-        <v>10</v>
-      </c>
-      <c r="D13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13">
-        <v>16.600000000000001</v>
-      </c>
-      <c r="F13">
-        <v>17.899999999999999</v>
-      </c>
-      <c r="G13">
-        <v>18.899999999999999</v>
-      </c>
-      <c r="H13">
-        <v>19.7</v>
-      </c>
-      <c r="I13">
-        <v>20.399999999999999</v>
-      </c>
-      <c r="J13">
-        <v>21.1</v>
-      </c>
-      <c r="K13">
-        <v>21.1</v>
-      </c>
-      <c r="L13">
-        <v>21.5</v>
-      </c>
-      <c r="M13">
-        <v>22</v>
-      </c>
-      <c r="N13">
-        <v>22.1</v>
-      </c>
-      <c r="O13">
-        <v>20.7</v>
-      </c>
-      <c r="P13">
-        <v>19.7</v>
-      </c>
-      <c r="Q13">
-        <v>19</v>
-      </c>
-      <c r="R13">
-        <v>18</v>
-      </c>
-      <c r="S13">
-        <v>17</v>
-      </c>
-      <c r="T13">
-        <v>17</v>
-      </c>
-      <c r="U13">
-        <v>16.7</v>
-      </c>
-      <c r="V13">
-        <v>16.600000000000001</v>
-      </c>
-      <c r="W13">
-        <v>16.100000000000001</v>
-      </c>
-      <c r="X13">
-        <v>16</v>
-      </c>
-      <c r="Y13">
-        <v>15.8</v>
-      </c>
-      <c r="Z13">
-        <v>15.5</v>
-      </c>
-      <c r="AA13">
-        <v>15.4</v>
-      </c>
-      <c r="AB13">
-        <v>15.2</v>
-      </c>
-      <c r="AC13">
-        <v>14.7</v>
-      </c>
-    </row>
-    <row r="20" spans="4:40" x14ac:dyDescent="0.2">
-      <c r="D20" s="21"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="23"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="23"/>
-      <c r="K20" s="22"/>
-      <c r="L20" s="23"/>
-      <c r="M20" s="22"/>
-      <c r="N20" s="23"/>
-      <c r="O20" s="22"/>
-      <c r="P20" s="23"/>
-      <c r="Q20" s="22"/>
-      <c r="R20" s="23"/>
-      <c r="S20" s="22"/>
-      <c r="T20" s="23"/>
-      <c r="U20" s="22"/>
-      <c r="V20" s="23"/>
-      <c r="W20" s="22"/>
-      <c r="X20" s="23"/>
-      <c r="Y20" s="22"/>
-      <c r="Z20" s="23"/>
-      <c r="AA20" s="22"/>
-      <c r="AB20" s="23"/>
-      <c r="AC20" s="22"/>
-      <c r="AD20" s="23"/>
-      <c r="AE20" s="22"/>
-      <c r="AF20" s="23"/>
-      <c r="AG20" s="22"/>
-      <c r="AH20" s="23"/>
-      <c r="AI20" s="22"/>
-      <c r="AJ20" s="23"/>
-      <c r="AK20" s="22"/>
-      <c r="AL20" s="23"/>
-      <c r="AM20" s="22"/>
-      <c r="AN20" s="27"/>
-    </row>
-  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Add data figure7 #257
</commit_message>
<xml_diff>
--- a/docs/housing_story_content/housing data story_part2.xlsx
+++ b/docs/housing_story_content/housing data story_part2.xlsx
@@ -17,7 +17,7 @@
     <sheet name="(17) housing vacancy" sheetId="22" r:id="rId3"/>
     <sheet name="(12) serviced zoned land" sheetId="11" r:id="rId4"/>
     <sheet name="(8) mortgages arrears" sheetId="7" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="33" r:id="rId6"/>
+    <sheet name="btl_mortgage_arrears" sheetId="33" r:id="rId6"/>
     <sheet name="(14) SH waiting list" sheetId="19" r:id="rId7"/>
     <sheet name="(20) PPPs housing ests" sheetId="25" r:id="rId8"/>
     <sheet name="(11) traveller accommodation" sheetId="10" r:id="rId9"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="318">
   <si>
     <t>Fingal</t>
   </si>
@@ -11963,7 +11963,7 @@
   <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="N40" sqref="N40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12604,13 +12604,16 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:P22"/>
+  <dimension ref="A2:P34"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="22.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
@@ -12876,7 +12879,7 @@
         <v>16514</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B17">
         <v>2013</v>
       </c>
@@ -12885,7 +12888,7 @@
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B18">
         <v>2016</v>
       </c>
@@ -12893,7 +12896,7 @@
         <v>91600</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B19">
         <v>2017</v>
       </c>
@@ -12902,7 +12905,7 @@
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B20">
         <v>2018</v>
       </c>
@@ -12910,8 +12913,242 @@
         <v>85799</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D22" s="1"/>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>317</v>
+      </c>
+      <c r="B22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" t="s">
+        <v>229</v>
+      </c>
+      <c r="D22" t="s">
+        <v>0</v>
+      </c>
+      <c r="E22" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>1991</v>
+      </c>
+      <c r="B23" s="1">
+        <v>20343</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>1993</v>
+      </c>
+      <c r="B24" s="1">
+        <v>28200</v>
+      </c>
+      <c r="C24">
+        <v>1119</v>
+      </c>
+      <c r="D24">
+        <v>810</v>
+      </c>
+      <c r="E24">
+        <v>809</v>
+      </c>
+      <c r="F24">
+        <v>5152</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>1996</v>
+      </c>
+      <c r="B25" s="1">
+        <v>27427</v>
+      </c>
+      <c r="C25">
+        <v>1209</v>
+      </c>
+      <c r="D25">
+        <v>666</v>
+      </c>
+      <c r="E25">
+        <v>702</v>
+      </c>
+      <c r="F25">
+        <v>3966</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>1999</v>
+      </c>
+      <c r="B26" s="1">
+        <v>39176</v>
+      </c>
+      <c r="C26">
+        <v>1363</v>
+      </c>
+      <c r="D26">
+        <v>1274</v>
+      </c>
+      <c r="E26">
+        <v>2396</v>
+      </c>
+      <c r="F26">
+        <v>6477</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>2002</v>
+      </c>
+      <c r="B27" s="1">
+        <v>48413</v>
+      </c>
+      <c r="C27">
+        <v>2118</v>
+      </c>
+      <c r="D27">
+        <v>1769</v>
+      </c>
+      <c r="E27">
+        <v>3817</v>
+      </c>
+      <c r="F27">
+        <v>6993</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>2005</v>
+      </c>
+      <c r="B28" s="1">
+        <v>43684</v>
+      </c>
+      <c r="C28">
+        <v>2319</v>
+      </c>
+      <c r="D28">
+        <v>1975</v>
+      </c>
+      <c r="E28">
+        <v>1656</v>
+      </c>
+      <c r="F28">
+        <v>5540</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>2008</v>
+      </c>
+      <c r="B29" s="1">
+        <v>56249</v>
+      </c>
+      <c r="C29">
+        <v>2461</v>
+      </c>
+      <c r="D29">
+        <v>1931</v>
+      </c>
+      <c r="E29">
+        <v>4259</v>
+      </c>
+      <c r="F29">
+        <v>4885</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>2011</v>
+      </c>
+      <c r="B30" s="1">
+        <v>98318</v>
+      </c>
+      <c r="C30">
+        <v>3909</v>
+      </c>
+      <c r="D30">
+        <v>5003</v>
+      </c>
+      <c r="E30">
+        <v>8022</v>
+      </c>
+      <c r="F30">
+        <v>8091</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>2013</v>
+      </c>
+      <c r="B31" s="1">
+        <v>89872</v>
+      </c>
+      <c r="C31" s="1">
+        <v>3406</v>
+      </c>
+      <c r="D31" s="1">
+        <v>6020</v>
+      </c>
+      <c r="E31" s="1">
+        <v>6217</v>
+      </c>
+      <c r="F31" s="1">
+        <v>16171</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>2016</v>
+      </c>
+      <c r="B32" s="1">
+        <v>91600</v>
+      </c>
+      <c r="C32" s="1">
+        <v>3341</v>
+      </c>
+      <c r="D32" s="1">
+        <v>6858</v>
+      </c>
+      <c r="E32" s="1">
+        <v>5562</v>
+      </c>
+      <c r="F32" s="1">
+        <v>19811</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>2017</v>
+      </c>
+      <c r="B33" s="1">
+        <v>71858</v>
+      </c>
+      <c r="C33" s="1"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>2018</v>
+      </c>
+      <c r="B34" s="1">
+        <v>85799</v>
+      </c>
+      <c r="C34" s="1">
+        <v>2843</v>
+      </c>
+      <c r="D34" s="1">
+        <v>6993</v>
+      </c>
+      <c r="E34" s="1">
+        <v>4846</v>
+      </c>
+      <c r="F34" s="1">
+        <v>16514</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13085,6 +13322,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="31.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="2:74" x14ac:dyDescent="0.2">
       <c r="C1" t="s">

</xml_diff>

<commit_message>
Add data figure8 #258
</commit_message>
<xml_diff>
--- a/docs/housing_story_content/housing data story_part2.xlsx
+++ b/docs/housing_story_content/housing data story_part2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="33600" windowHeight="18940" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Part 2 charts summary" sheetId="32" r:id="rId1"/>
@@ -18,10 +18,11 @@
     <sheet name="(12) serviced zoned land" sheetId="11" r:id="rId4"/>
     <sheet name="(8) mortgages arrears" sheetId="7" r:id="rId5"/>
     <sheet name="btl_mortgage_arrears" sheetId="33" r:id="rId6"/>
-    <sheet name="(14) SH waiting list" sheetId="19" r:id="rId7"/>
-    <sheet name="(20) PPPs housing ests" sheetId="25" r:id="rId8"/>
-    <sheet name="(11) traveller accommodation" sheetId="10" r:id="rId9"/>
-    <sheet name="(9) BTL arrears" sheetId="8" r:id="rId10"/>
+    <sheet name="rent_supplement" sheetId="34" r:id="rId7"/>
+    <sheet name="(14) SH waiting list" sheetId="19" r:id="rId8"/>
+    <sheet name="(20) PPPs housing ests" sheetId="25" r:id="rId9"/>
+    <sheet name="(11) traveller accommodation" sheetId="10" r:id="rId10"/>
+    <sheet name="(9) BTL arrears" sheetId="8" r:id="rId11"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -1060,7 +1061,7 @@
     <numFmt numFmtId="168" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;?_-;_-@_-"/>
     <numFmt numFmtId="169" formatCode="0.0"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1215,8 +1216,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1258,8 +1272,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA6A6A6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="40">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -1726,6 +1752,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFA6A6A6"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFA6A6A6"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="733">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2462,7 +2527,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2655,6 +2720,21 @@
     </xf>
     <xf numFmtId="3" fontId="10" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="22" fillId="8" borderId="40" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="22" fillId="8" borderId="41" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="22" fillId="8" borderId="41" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="42" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="733">
@@ -3904,6 +3984,1249 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:BV24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="31.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:74" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="3" spans="2:74" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="33"/>
+      <c r="C3" s="97" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
+      <c r="L3" s="97"/>
+      <c r="M3" s="97"/>
+      <c r="N3" s="97"/>
+      <c r="O3" s="97"/>
+      <c r="P3" s="97"/>
+      <c r="Q3" s="97"/>
+      <c r="R3" s="97"/>
+      <c r="S3" s="97"/>
+      <c r="T3" s="97"/>
+      <c r="U3" s="97"/>
+      <c r="V3" s="97"/>
+      <c r="W3" s="97"/>
+      <c r="X3" s="97"/>
+      <c r="Y3" s="97"/>
+      <c r="Z3" s="97"/>
+    </row>
+    <row r="4" spans="2:74" ht="16" x14ac:dyDescent="0.2">
+      <c r="B4" s="98" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="100" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="100"/>
+      <c r="E4" s="100"/>
+      <c r="F4" s="100"/>
+      <c r="G4" s="100"/>
+      <c r="H4" s="100"/>
+      <c r="I4" s="100"/>
+      <c r="J4" s="100"/>
+      <c r="K4" s="100"/>
+      <c r="L4" s="100"/>
+      <c r="M4" s="100"/>
+      <c r="N4" s="101"/>
+      <c r="O4" s="102" t="s">
+        <v>27</v>
+      </c>
+      <c r="P4" s="100"/>
+      <c r="Q4" s="100"/>
+      <c r="R4" s="100"/>
+      <c r="S4" s="100"/>
+      <c r="T4" s="100"/>
+      <c r="U4" s="100"/>
+      <c r="V4" s="100"/>
+      <c r="W4" s="100"/>
+      <c r="X4" s="100"/>
+      <c r="Y4" s="100"/>
+      <c r="Z4" s="101"/>
+    </row>
+    <row r="5" spans="2:74" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="99"/>
+      <c r="C5" s="34">
+        <v>2002</v>
+      </c>
+      <c r="D5" s="34">
+        <v>2003</v>
+      </c>
+      <c r="E5" s="34">
+        <v>2004</v>
+      </c>
+      <c r="F5" s="34">
+        <v>2005</v>
+      </c>
+      <c r="G5" s="34">
+        <v>2006</v>
+      </c>
+      <c r="H5" s="34">
+        <v>2007</v>
+      </c>
+      <c r="I5" s="34">
+        <v>2008</v>
+      </c>
+      <c r="J5" s="34">
+        <v>2009</v>
+      </c>
+      <c r="K5" s="34">
+        <v>2010</v>
+      </c>
+      <c r="L5" s="34">
+        <v>2011</v>
+      </c>
+      <c r="M5" s="34">
+        <v>2012</v>
+      </c>
+      <c r="N5" s="35">
+        <v>2013</v>
+      </c>
+      <c r="O5" s="36">
+        <v>2002</v>
+      </c>
+      <c r="P5" s="34">
+        <v>2003</v>
+      </c>
+      <c r="Q5" s="34">
+        <v>2004</v>
+      </c>
+      <c r="R5" s="34">
+        <v>2005</v>
+      </c>
+      <c r="S5" s="34">
+        <v>2006</v>
+      </c>
+      <c r="T5" s="34">
+        <v>2007</v>
+      </c>
+      <c r="U5" s="34">
+        <v>2008</v>
+      </c>
+      <c r="V5" s="34">
+        <v>2009</v>
+      </c>
+      <c r="W5" s="34">
+        <v>2010</v>
+      </c>
+      <c r="X5" s="34">
+        <v>2011</v>
+      </c>
+      <c r="Y5" s="34">
+        <v>2012</v>
+      </c>
+      <c r="Z5" s="35">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="6" spans="2:74" ht="16" x14ac:dyDescent="0.2">
+      <c r="B6" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="38">
+        <v>97</v>
+      </c>
+      <c r="D6" s="38">
+        <v>110</v>
+      </c>
+      <c r="E6" s="38">
+        <v>90</v>
+      </c>
+      <c r="F6" s="38">
+        <v>94</v>
+      </c>
+      <c r="G6" s="38">
+        <v>91</v>
+      </c>
+      <c r="H6" s="39">
+        <v>87</v>
+      </c>
+      <c r="I6" s="39">
+        <v>85</v>
+      </c>
+      <c r="J6" s="40">
+        <v>95</v>
+      </c>
+      <c r="K6" s="40">
+        <v>92</v>
+      </c>
+      <c r="L6" s="40">
+        <v>97</v>
+      </c>
+      <c r="M6" s="40">
+        <v>89</v>
+      </c>
+      <c r="N6" s="41">
+        <v>94</v>
+      </c>
+      <c r="O6" s="42">
+        <v>15</v>
+      </c>
+      <c r="P6" s="38">
+        <v>10</v>
+      </c>
+      <c r="Q6" s="38">
+        <v>11</v>
+      </c>
+      <c r="R6" s="38">
+        <v>12</v>
+      </c>
+      <c r="S6" s="38">
+        <v>5</v>
+      </c>
+      <c r="T6" s="38">
+        <v>3</v>
+      </c>
+      <c r="U6" s="38">
+        <v>0</v>
+      </c>
+      <c r="V6" s="43">
+        <v>2</v>
+      </c>
+      <c r="W6" s="43">
+        <v>2</v>
+      </c>
+      <c r="X6" s="43">
+        <v>3</v>
+      </c>
+      <c r="Y6" s="43">
+        <v>3</v>
+      </c>
+      <c r="Z6" s="44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:74" ht="16" x14ac:dyDescent="0.2">
+      <c r="B7" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="38">
+        <v>249</v>
+      </c>
+      <c r="D7" s="38">
+        <v>267</v>
+      </c>
+      <c r="E7" s="38">
+        <v>257</v>
+      </c>
+      <c r="F7" s="38">
+        <v>218</v>
+      </c>
+      <c r="G7" s="38">
+        <v>190</v>
+      </c>
+      <c r="H7" s="39">
+        <v>209</v>
+      </c>
+      <c r="I7" s="39">
+        <v>216</v>
+      </c>
+      <c r="J7" s="40">
+        <v>196</v>
+      </c>
+      <c r="K7" s="40">
+        <v>194</v>
+      </c>
+      <c r="L7" s="40">
+        <v>192</v>
+      </c>
+      <c r="M7" s="40">
+        <v>200</v>
+      </c>
+      <c r="N7" s="41">
+        <v>213</v>
+      </c>
+      <c r="O7" s="42">
+        <v>35</v>
+      </c>
+      <c r="P7" s="38">
+        <v>15</v>
+      </c>
+      <c r="Q7" s="38">
+        <v>7</v>
+      </c>
+      <c r="R7" s="38">
+        <v>43</v>
+      </c>
+      <c r="S7" s="38">
+        <v>66</v>
+      </c>
+      <c r="T7" s="38">
+        <v>74</v>
+      </c>
+      <c r="U7" s="38">
+        <v>42</v>
+      </c>
+      <c r="V7" s="43">
+        <v>43</v>
+      </c>
+      <c r="W7" s="43">
+        <v>45</v>
+      </c>
+      <c r="X7" s="43">
+        <v>33</v>
+      </c>
+      <c r="Y7" s="43">
+        <v>28</v>
+      </c>
+      <c r="Z7" s="44">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="2:74" ht="16" x14ac:dyDescent="0.2">
+      <c r="B8" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="38">
+        <v>54</v>
+      </c>
+      <c r="D8" s="38">
+        <v>62</v>
+      </c>
+      <c r="E8" s="38">
+        <v>56</v>
+      </c>
+      <c r="F8" s="38">
+        <v>67</v>
+      </c>
+      <c r="G8" s="38">
+        <v>75</v>
+      </c>
+      <c r="H8" s="39">
+        <v>82</v>
+      </c>
+      <c r="I8" s="39">
+        <v>79</v>
+      </c>
+      <c r="J8" s="40">
+        <v>70</v>
+      </c>
+      <c r="K8" s="40">
+        <v>68</v>
+      </c>
+      <c r="L8" s="40">
+        <v>69</v>
+      </c>
+      <c r="M8" s="40">
+        <v>58</v>
+      </c>
+      <c r="N8" s="41">
+        <v>64</v>
+      </c>
+      <c r="O8" s="42">
+        <v>50</v>
+      </c>
+      <c r="P8" s="38">
+        <v>16</v>
+      </c>
+      <c r="Q8" s="38">
+        <v>28</v>
+      </c>
+      <c r="R8" s="38">
+        <v>20</v>
+      </c>
+      <c r="S8" s="38">
+        <v>10</v>
+      </c>
+      <c r="T8" s="38">
+        <v>16</v>
+      </c>
+      <c r="U8" s="38">
+        <v>17</v>
+      </c>
+      <c r="V8" s="43">
+        <v>22</v>
+      </c>
+      <c r="W8" s="43">
+        <v>8</v>
+      </c>
+      <c r="X8" s="43">
+        <v>7</v>
+      </c>
+      <c r="Y8" s="43">
+        <v>9</v>
+      </c>
+      <c r="Z8" s="44">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="2:74" ht="16" x14ac:dyDescent="0.2">
+      <c r="B9" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="38">
+        <v>157</v>
+      </c>
+      <c r="D9" s="38">
+        <v>175</v>
+      </c>
+      <c r="E9" s="38">
+        <v>173</v>
+      </c>
+      <c r="F9" s="38">
+        <v>178</v>
+      </c>
+      <c r="G9" s="38">
+        <v>151</v>
+      </c>
+      <c r="H9" s="39">
+        <v>159</v>
+      </c>
+      <c r="I9" s="39">
+        <v>158</v>
+      </c>
+      <c r="J9" s="40">
+        <v>156</v>
+      </c>
+      <c r="K9" s="40">
+        <v>154</v>
+      </c>
+      <c r="L9" s="40">
+        <v>175</v>
+      </c>
+      <c r="M9" s="40">
+        <v>177</v>
+      </c>
+      <c r="N9" s="41">
+        <v>179</v>
+      </c>
+      <c r="O9" s="42">
+        <v>1</v>
+      </c>
+      <c r="P9" s="38">
+        <v>4</v>
+      </c>
+      <c r="Q9" s="38">
+        <v>4</v>
+      </c>
+      <c r="R9" s="38">
+        <v>0</v>
+      </c>
+      <c r="S9" s="38">
+        <v>6</v>
+      </c>
+      <c r="T9" s="38">
+        <v>6</v>
+      </c>
+      <c r="U9" s="38">
+        <v>12</v>
+      </c>
+      <c r="V9" s="43">
+        <v>2</v>
+      </c>
+      <c r="W9" s="43">
+        <v>10</v>
+      </c>
+      <c r="X9" s="43">
+        <v>9</v>
+      </c>
+      <c r="Y9" s="43">
+        <v>10</v>
+      </c>
+      <c r="Z9" s="44">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="2:74" ht="16" x14ac:dyDescent="0.2">
+      <c r="B10" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="38">
+        <v>370</v>
+      </c>
+      <c r="D10" s="38">
+        <v>402</v>
+      </c>
+      <c r="E10" s="38">
+        <v>394</v>
+      </c>
+      <c r="F10" s="38">
+        <v>381</v>
+      </c>
+      <c r="G10" s="38">
+        <v>394</v>
+      </c>
+      <c r="H10" s="39">
+        <v>417</v>
+      </c>
+      <c r="I10" s="39">
+        <v>408</v>
+      </c>
+      <c r="J10" s="40">
+        <v>425</v>
+      </c>
+      <c r="K10" s="40">
+        <v>356</v>
+      </c>
+      <c r="L10" s="40">
+        <v>303</v>
+      </c>
+      <c r="M10" s="40">
+        <v>291</v>
+      </c>
+      <c r="N10" s="41">
+        <v>295</v>
+      </c>
+      <c r="O10" s="42">
+        <v>31</v>
+      </c>
+      <c r="P10" s="38">
+        <v>29</v>
+      </c>
+      <c r="Q10" s="38">
+        <v>4</v>
+      </c>
+      <c r="R10" s="38">
+        <v>15</v>
+      </c>
+      <c r="S10" s="38">
+        <v>19</v>
+      </c>
+      <c r="T10" s="38">
+        <v>7</v>
+      </c>
+      <c r="U10" s="38">
+        <v>10</v>
+      </c>
+      <c r="V10" s="43">
+        <v>0</v>
+      </c>
+      <c r="W10" s="43">
+        <v>0</v>
+      </c>
+      <c r="X10" s="43">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="43">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:74" ht="16" x14ac:dyDescent="0.2">
+      <c r="B11" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="38">
+        <v>99</v>
+      </c>
+      <c r="D11" s="38">
+        <v>111</v>
+      </c>
+      <c r="E11" s="38">
+        <v>113</v>
+      </c>
+      <c r="F11" s="38">
+        <v>119</v>
+      </c>
+      <c r="G11" s="38">
+        <v>125</v>
+      </c>
+      <c r="H11" s="39">
+        <v>142</v>
+      </c>
+      <c r="I11" s="39">
+        <v>152</v>
+      </c>
+      <c r="J11" s="40">
+        <v>157</v>
+      </c>
+      <c r="K11" s="40">
+        <v>162</v>
+      </c>
+      <c r="L11" s="40">
+        <v>164</v>
+      </c>
+      <c r="M11" s="40">
+        <v>169</v>
+      </c>
+      <c r="N11" s="41">
+        <v>165</v>
+      </c>
+      <c r="O11" s="42">
+        <v>29</v>
+      </c>
+      <c r="P11" s="38">
+        <v>32</v>
+      </c>
+      <c r="Q11" s="38">
+        <v>23</v>
+      </c>
+      <c r="R11" s="38">
+        <v>35</v>
+      </c>
+      <c r="S11" s="38">
+        <v>27</v>
+      </c>
+      <c r="T11" s="38">
+        <v>26</v>
+      </c>
+      <c r="U11" s="38">
+        <v>16</v>
+      </c>
+      <c r="V11" s="43">
+        <v>8</v>
+      </c>
+      <c r="W11" s="43">
+        <v>4</v>
+      </c>
+      <c r="X11" s="43">
+        <v>4</v>
+      </c>
+      <c r="Y11" s="43">
+        <v>2</v>
+      </c>
+      <c r="Z11" s="44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:74" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="38">
+        <v>393</v>
+      </c>
+      <c r="D12" s="38">
+        <v>429</v>
+      </c>
+      <c r="E12" s="38">
+        <v>434</v>
+      </c>
+      <c r="F12" s="38">
+        <v>445</v>
+      </c>
+      <c r="G12" s="38">
+        <v>451</v>
+      </c>
+      <c r="H12" s="39">
+        <v>441</v>
+      </c>
+      <c r="I12" s="39">
+        <v>437</v>
+      </c>
+      <c r="J12" s="40">
+        <v>446</v>
+      </c>
+      <c r="K12" s="40">
+        <v>447</v>
+      </c>
+      <c r="L12" s="40">
+        <v>456</v>
+      </c>
+      <c r="M12" s="40">
+        <v>459</v>
+      </c>
+      <c r="N12" s="41">
+        <v>466</v>
+      </c>
+      <c r="O12" s="42">
+        <v>62</v>
+      </c>
+      <c r="P12" s="38">
+        <v>71</v>
+      </c>
+      <c r="Q12" s="38">
+        <v>41</v>
+      </c>
+      <c r="R12" s="38">
+        <v>72</v>
+      </c>
+      <c r="S12" s="38">
+        <v>70</v>
+      </c>
+      <c r="T12" s="38">
+        <v>46</v>
+      </c>
+      <c r="U12" s="38">
+        <v>64</v>
+      </c>
+      <c r="V12" s="43">
+        <v>55</v>
+      </c>
+      <c r="W12" s="43">
+        <v>73</v>
+      </c>
+      <c r="X12" s="43">
+        <v>48</v>
+      </c>
+      <c r="Y12" s="43">
+        <v>25</v>
+      </c>
+      <c r="Z12" s="44">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="2:74" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="46">
+        <v>4522</v>
+      </c>
+      <c r="D13" s="46">
+        <v>4952</v>
+      </c>
+      <c r="E13" s="46">
+        <v>5106</v>
+      </c>
+      <c r="F13" s="46">
+        <v>5177</v>
+      </c>
+      <c r="G13" s="46">
+        <v>5251</v>
+      </c>
+      <c r="H13" s="47">
+        <v>5436</v>
+      </c>
+      <c r="I13" s="47">
+        <v>5500</v>
+      </c>
+      <c r="J13" s="47">
+        <v>5617</v>
+      </c>
+      <c r="K13" s="47">
+        <v>5634</v>
+      </c>
+      <c r="L13" s="47">
+        <v>5595</v>
+      </c>
+      <c r="M13" s="47">
+        <v>5568</v>
+      </c>
+      <c r="N13" s="48">
+        <v>5574</v>
+      </c>
+      <c r="O13" s="49">
+        <v>939</v>
+      </c>
+      <c r="P13" s="46">
+        <v>788</v>
+      </c>
+      <c r="Q13" s="46">
+        <v>601</v>
+      </c>
+      <c r="R13" s="46">
+        <v>589</v>
+      </c>
+      <c r="S13" s="46">
+        <v>629</v>
+      </c>
+      <c r="T13" s="46">
+        <v>594</v>
+      </c>
+      <c r="U13" s="46">
+        <v>524</v>
+      </c>
+      <c r="V13" s="46">
+        <v>422</v>
+      </c>
+      <c r="W13" s="46">
+        <v>444</v>
+      </c>
+      <c r="X13" s="46">
+        <v>327</v>
+      </c>
+      <c r="Y13" s="46">
+        <v>330</v>
+      </c>
+      <c r="Z13" s="50">
+        <v>361</v>
+      </c>
+      <c r="AA13">
+        <v>417</v>
+      </c>
+      <c r="AB13">
+        <v>443</v>
+      </c>
+      <c r="AC13">
+        <v>464</v>
+      </c>
+      <c r="AD13">
+        <v>478</v>
+      </c>
+      <c r="AE13">
+        <v>485</v>
+      </c>
+      <c r="AF13">
+        <v>489</v>
+      </c>
+      <c r="AG13">
+        <v>513</v>
+      </c>
+      <c r="AH13">
+        <v>511</v>
+      </c>
+      <c r="AI13">
+        <v>561</v>
+      </c>
+      <c r="AJ13">
+        <v>563</v>
+      </c>
+      <c r="AK13">
+        <v>580</v>
+      </c>
+      <c r="AL13">
+        <v>584</v>
+      </c>
+      <c r="AM13">
+        <v>162</v>
+      </c>
+      <c r="AN13">
+        <v>293</v>
+      </c>
+      <c r="AO13">
+        <v>486</v>
+      </c>
+      <c r="AP13">
+        <v>696</v>
+      </c>
+      <c r="AQ13">
+        <v>935</v>
+      </c>
+      <c r="AR13" s="1">
+        <v>1143</v>
+      </c>
+      <c r="AS13" s="1">
+        <v>1516</v>
+      </c>
+      <c r="AT13" s="1">
+        <v>2003</v>
+      </c>
+      <c r="AU13" s="1">
+        <v>2380</v>
+      </c>
+      <c r="AV13" s="1">
+        <v>2558</v>
+      </c>
+      <c r="AW13" s="1">
+        <v>2829</v>
+      </c>
+      <c r="AX13" s="1">
+        <v>2717</v>
+      </c>
+      <c r="AY13">
+        <v>249</v>
+      </c>
+      <c r="AZ13">
+        <v>323</v>
+      </c>
+      <c r="BA13">
+        <v>334</v>
+      </c>
+      <c r="BB13">
+        <v>326</v>
+      </c>
+      <c r="BC13">
+        <v>391</v>
+      </c>
+      <c r="BD13">
+        <v>437</v>
+      </c>
+      <c r="BE13">
+        <v>345</v>
+      </c>
+      <c r="BF13">
+        <v>390</v>
+      </c>
+      <c r="BG13">
+        <v>451</v>
+      </c>
+      <c r="BH13">
+        <v>492</v>
+      </c>
+      <c r="BI13">
+        <v>604</v>
+      </c>
+      <c r="BJ13">
+        <v>663</v>
+      </c>
+      <c r="BK13" s="1">
+        <v>6289</v>
+      </c>
+      <c r="BL13" s="1">
+        <v>6799</v>
+      </c>
+      <c r="BM13" s="1">
+        <v>6991</v>
+      </c>
+      <c r="BN13" s="1">
+        <v>7266</v>
+      </c>
+      <c r="BO13" s="1">
+        <v>7691</v>
+      </c>
+      <c r="BP13" s="1">
+        <v>8099</v>
+      </c>
+      <c r="BQ13" s="1">
+        <v>8398</v>
+      </c>
+      <c r="BR13" s="1">
+        <v>8943</v>
+      </c>
+      <c r="BS13" s="1">
+        <v>9470</v>
+      </c>
+      <c r="BT13" s="1">
+        <v>9535</v>
+      </c>
+      <c r="BU13" s="1">
+        <v>9911</v>
+      </c>
+      <c r="BV13" s="1">
+        <v>9899</v>
+      </c>
+    </row>
+    <row r="14" spans="2:74" ht="16" x14ac:dyDescent="0.2">
+      <c r="B14" s="51"/>
+      <c r="C14" s="51"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="51"/>
+      <c r="G14" s="51"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="52"/>
+      <c r="J14" s="52"/>
+      <c r="K14" s="52"/>
+      <c r="L14" s="52"/>
+      <c r="M14" s="52"/>
+      <c r="N14" s="52"/>
+      <c r="O14" s="51"/>
+      <c r="P14" s="51"/>
+      <c r="Q14" s="51"/>
+      <c r="R14" s="51"/>
+      <c r="S14" s="51"/>
+      <c r="T14" s="51"/>
+      <c r="U14" s="51"/>
+      <c r="V14" s="51"/>
+      <c r="W14" s="51"/>
+      <c r="X14" s="51"/>
+      <c r="Y14" s="51"/>
+      <c r="Z14" s="51"/>
+    </row>
+    <row r="15" spans="2:74" ht="16" x14ac:dyDescent="0.2">
+      <c r="B15" s="51" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="51"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="51"/>
+      <c r="F15" s="51"/>
+      <c r="G15" s="51"/>
+      <c r="H15" s="52"/>
+      <c r="I15" s="52"/>
+      <c r="J15" s="52"/>
+      <c r="K15" s="52"/>
+      <c r="L15" s="52"/>
+      <c r="M15" s="52"/>
+      <c r="N15" s="52"/>
+      <c r="O15" s="51"/>
+      <c r="P15" s="51"/>
+      <c r="Q15" s="51"/>
+      <c r="R15" s="51"/>
+      <c r="S15" s="51"/>
+      <c r="T15" s="51"/>
+      <c r="U15" s="51"/>
+      <c r="V15" s="51"/>
+      <c r="W15" s="51"/>
+      <c r="X15" s="51"/>
+      <c r="Y15" s="51"/>
+      <c r="Z15" s="51"/>
+    </row>
+    <row r="16" spans="2:74" ht="16" x14ac:dyDescent="0.2">
+      <c r="B16" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="51"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="51"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="52"/>
+      <c r="K16" s="52"/>
+      <c r="L16" s="52"/>
+      <c r="M16" s="52"/>
+      <c r="N16" s="52"/>
+      <c r="O16" s="51"/>
+      <c r="P16" s="51"/>
+      <c r="Q16" s="51"/>
+      <c r="R16" s="51"/>
+      <c r="S16" s="51"/>
+      <c r="T16" s="51"/>
+      <c r="U16" s="51"/>
+      <c r="V16" s="51"/>
+      <c r="W16" s="51"/>
+      <c r="X16" s="51"/>
+      <c r="Y16" s="51"/>
+      <c r="Z16" s="51"/>
+    </row>
+    <row r="17" spans="2:26" ht="16" x14ac:dyDescent="0.2">
+      <c r="B17" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="51"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="51"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="51"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="52"/>
+      <c r="J17" s="52"/>
+      <c r="K17" s="52"/>
+      <c r="L17" s="52"/>
+      <c r="M17" s="52"/>
+      <c r="N17" s="52"/>
+      <c r="O17" s="51"/>
+      <c r="P17" s="51"/>
+      <c r="Q17" s="51"/>
+      <c r="R17" s="51"/>
+      <c r="S17" s="51"/>
+      <c r="T17" s="51"/>
+      <c r="U17" s="51"/>
+      <c r="V17" s="51"/>
+      <c r="W17" s="51"/>
+      <c r="X17" s="51"/>
+      <c r="Y17" s="51"/>
+      <c r="Z17" s="51"/>
+    </row>
+    <row r="18" spans="2:26" ht="16" x14ac:dyDescent="0.2">
+      <c r="B18" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="51"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="51"/>
+      <c r="H18" s="52"/>
+      <c r="I18" s="52"/>
+      <c r="J18" s="52"/>
+      <c r="K18" s="52"/>
+      <c r="L18" s="52"/>
+      <c r="M18" s="52"/>
+      <c r="N18" s="52"/>
+      <c r="O18" s="51"/>
+      <c r="P18" s="51"/>
+      <c r="Q18" s="51"/>
+      <c r="R18" s="51"/>
+      <c r="S18" s="51"/>
+      <c r="T18" s="51"/>
+      <c r="U18" s="51"/>
+      <c r="V18" s="51"/>
+      <c r="W18" s="51"/>
+      <c r="X18" s="51"/>
+      <c r="Y18" s="51"/>
+      <c r="Z18" s="51"/>
+    </row>
+    <row r="19" spans="2:26" ht="16" x14ac:dyDescent="0.2">
+      <c r="B19" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="53"/>
+      <c r="D19" s="53"/>
+      <c r="E19" s="53"/>
+      <c r="F19" s="53"/>
+      <c r="G19" s="53"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="39"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="39"/>
+      <c r="L19" s="39"/>
+      <c r="M19" s="39"/>
+      <c r="N19" s="39"/>
+      <c r="O19" s="53"/>
+      <c r="P19" s="53"/>
+      <c r="Q19" s="53"/>
+      <c r="R19" s="53"/>
+      <c r="S19" s="53"/>
+      <c r="T19" s="53"/>
+      <c r="U19" s="53"/>
+      <c r="V19" s="53"/>
+      <c r="W19" s="53"/>
+      <c r="X19" s="53"/>
+      <c r="Y19" s="53"/>
+      <c r="Z19" s="53"/>
+    </row>
+    <row r="20" spans="2:26" ht="16" x14ac:dyDescent="0.2">
+      <c r="B20" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="53"/>
+      <c r="D20" s="53"/>
+      <c r="E20" s="53"/>
+      <c r="F20" s="53"/>
+      <c r="G20" s="53"/>
+      <c r="H20" s="39"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
+      <c r="K20" s="39"/>
+      <c r="L20" s="39"/>
+      <c r="M20" s="39"/>
+      <c r="N20" s="39"/>
+      <c r="O20" s="53"/>
+      <c r="P20" s="53"/>
+      <c r="Q20" s="53"/>
+      <c r="R20" s="53"/>
+      <c r="S20" s="53"/>
+      <c r="T20" s="53"/>
+      <c r="U20" s="53"/>
+      <c r="V20" s="53"/>
+      <c r="W20" s="53"/>
+      <c r="X20" s="53"/>
+      <c r="Y20" s="53"/>
+      <c r="Z20" s="53"/>
+    </row>
+    <row r="21" spans="2:26" ht="16" x14ac:dyDescent="0.2">
+      <c r="B21" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="53"/>
+      <c r="D21" s="53"/>
+      <c r="E21" s="53"/>
+      <c r="F21" s="53"/>
+      <c r="G21" s="53"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="39"/>
+      <c r="J21" s="39"/>
+      <c r="K21" s="39"/>
+      <c r="L21" s="39"/>
+      <c r="M21" s="39"/>
+      <c r="N21" s="39"/>
+      <c r="O21" s="53"/>
+      <c r="P21" s="53"/>
+      <c r="Q21" s="53"/>
+      <c r="R21" s="53"/>
+      <c r="S21" s="53"/>
+      <c r="T21" s="53"/>
+      <c r="U21" s="53"/>
+      <c r="V21" s="53"/>
+      <c r="W21" s="53"/>
+      <c r="X21" s="53"/>
+      <c r="Y21" s="53"/>
+      <c r="Z21" s="53"/>
+    </row>
+    <row r="22" spans="2:26" ht="16" x14ac:dyDescent="0.2">
+      <c r="B22" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="53"/>
+      <c r="D22" s="53"/>
+      <c r="E22" s="53"/>
+      <c r="F22" s="53"/>
+      <c r="G22" s="53"/>
+      <c r="H22" s="39"/>
+      <c r="I22" s="39"/>
+      <c r="J22" s="39"/>
+      <c r="K22" s="39"/>
+      <c r="L22" s="39"/>
+      <c r="M22" s="39"/>
+      <c r="N22" s="39"/>
+      <c r="O22" s="53"/>
+      <c r="P22" s="53"/>
+      <c r="Q22" s="53"/>
+      <c r="R22" s="53"/>
+      <c r="S22" s="53"/>
+      <c r="T22" s="53"/>
+      <c r="U22" s="53"/>
+      <c r="V22" s="53"/>
+      <c r="W22" s="53"/>
+      <c r="X22" s="53"/>
+      <c r="Y22" s="53"/>
+      <c r="Z22" s="53"/>
+    </row>
+    <row r="23" spans="2:26" ht="16" x14ac:dyDescent="0.2">
+      <c r="B23" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="53"/>
+      <c r="D23" s="53"/>
+      <c r="E23" s="53"/>
+      <c r="F23" s="53"/>
+      <c r="G23" s="53"/>
+      <c r="H23" s="39"/>
+      <c r="I23" s="39"/>
+      <c r="J23" s="39"/>
+      <c r="K23" s="39"/>
+      <c r="L23" s="39"/>
+      <c r="M23" s="39"/>
+      <c r="N23" s="39"/>
+      <c r="O23" s="53"/>
+      <c r="P23" s="53"/>
+      <c r="Q23" s="53"/>
+      <c r="R23" s="53"/>
+      <c r="S23" s="53"/>
+      <c r="T23" s="53"/>
+      <c r="U23" s="53"/>
+      <c r="V23" s="53"/>
+      <c r="W23" s="53"/>
+      <c r="X23" s="53"/>
+      <c r="Y23" s="53"/>
+      <c r="Z23" s="53"/>
+    </row>
+    <row r="24" spans="2:26" ht="16" x14ac:dyDescent="0.2">
+      <c r="B24" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="53"/>
+      <c r="D24" s="53"/>
+      <c r="E24" s="53"/>
+      <c r="F24" s="53"/>
+      <c r="G24" s="53"/>
+      <c r="H24" s="53"/>
+      <c r="I24" s="53"/>
+      <c r="J24" s="53"/>
+      <c r="K24" s="53"/>
+      <c r="L24" s="53"/>
+      <c r="M24" s="53"/>
+      <c r="N24" s="53"/>
+      <c r="O24" s="53"/>
+      <c r="P24" s="53"/>
+      <c r="Q24" s="53"/>
+      <c r="R24" s="53"/>
+      <c r="S24" s="53"/>
+      <c r="T24" s="53"/>
+      <c r="U24" s="53"/>
+      <c r="V24" s="53"/>
+      <c r="W24" s="53"/>
+      <c r="X24" s="53"/>
+      <c r="Y24" s="53"/>
+      <c r="Z24" s="53"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C3:Z3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:N4"/>
+    <mergeCell ref="O4:Z4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:AN20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11962,7 +13285,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N40" sqref="N40"/>
     </sheetView>
   </sheetViews>
@@ -12603,6 +13926,109 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="106">
+        <v>2008</v>
+      </c>
+      <c r="B1" s="103">
+        <v>74038</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="106">
+        <v>2009</v>
+      </c>
+      <c r="B2" s="104">
+        <v>93030</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="106">
+        <v>2010</v>
+      </c>
+      <c r="B3" s="104">
+        <v>97260</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="106">
+        <v>2011</v>
+      </c>
+      <c r="B4" s="104">
+        <v>96803</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="106">
+        <v>2012</v>
+      </c>
+      <c r="B5" s="104">
+        <v>87684</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="106">
+        <v>2013</v>
+      </c>
+      <c r="B6" s="104">
+        <v>79788</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="106">
+        <v>2014</v>
+      </c>
+      <c r="B7" s="104">
+        <v>66409</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="106">
+        <v>2015</v>
+      </c>
+      <c r="B8" s="104">
+        <v>56959</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="106">
+        <v>2016</v>
+      </c>
+      <c r="B9" s="104">
+        <v>44521</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="106">
+        <v>2017</v>
+      </c>
+      <c r="B10" s="104">
+        <v>32075</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="107">
+        <v>2018</v>
+      </c>
+      <c r="B11" s="105">
+        <v>22880</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:P34"/>
   <sheetViews>
@@ -13155,7 +14581,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E13"/>
   <sheetViews>
@@ -13309,1249 +14735,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:BV24"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="31.1640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:74" x14ac:dyDescent="0.2">
-      <c r="C1" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="3" spans="2:74" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="33"/>
-      <c r="C3" s="97" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-      <c r="K3" s="97"/>
-      <c r="L3" s="97"/>
-      <c r="M3" s="97"/>
-      <c r="N3" s="97"/>
-      <c r="O3" s="97"/>
-      <c r="P3" s="97"/>
-      <c r="Q3" s="97"/>
-      <c r="R3" s="97"/>
-      <c r="S3" s="97"/>
-      <c r="T3" s="97"/>
-      <c r="U3" s="97"/>
-      <c r="V3" s="97"/>
-      <c r="W3" s="97"/>
-      <c r="X3" s="97"/>
-      <c r="Y3" s="97"/>
-      <c r="Z3" s="97"/>
-    </row>
-    <row r="4" spans="2:74" ht="16" x14ac:dyDescent="0.2">
-      <c r="B4" s="98" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="100" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="100"/>
-      <c r="E4" s="100"/>
-      <c r="F4" s="100"/>
-      <c r="G4" s="100"/>
-      <c r="H4" s="100"/>
-      <c r="I4" s="100"/>
-      <c r="J4" s="100"/>
-      <c r="K4" s="100"/>
-      <c r="L4" s="100"/>
-      <c r="M4" s="100"/>
-      <c r="N4" s="101"/>
-      <c r="O4" s="102" t="s">
-        <v>27</v>
-      </c>
-      <c r="P4" s="100"/>
-      <c r="Q4" s="100"/>
-      <c r="R4" s="100"/>
-      <c r="S4" s="100"/>
-      <c r="T4" s="100"/>
-      <c r="U4" s="100"/>
-      <c r="V4" s="100"/>
-      <c r="W4" s="100"/>
-      <c r="X4" s="100"/>
-      <c r="Y4" s="100"/>
-      <c r="Z4" s="101"/>
-    </row>
-    <row r="5" spans="2:74" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="99"/>
-      <c r="C5" s="34">
-        <v>2002</v>
-      </c>
-      <c r="D5" s="34">
-        <v>2003</v>
-      </c>
-      <c r="E5" s="34">
-        <v>2004</v>
-      </c>
-      <c r="F5" s="34">
-        <v>2005</v>
-      </c>
-      <c r="G5" s="34">
-        <v>2006</v>
-      </c>
-      <c r="H5" s="34">
-        <v>2007</v>
-      </c>
-      <c r="I5" s="34">
-        <v>2008</v>
-      </c>
-      <c r="J5" s="34">
-        <v>2009</v>
-      </c>
-      <c r="K5" s="34">
-        <v>2010</v>
-      </c>
-      <c r="L5" s="34">
-        <v>2011</v>
-      </c>
-      <c r="M5" s="34">
-        <v>2012</v>
-      </c>
-      <c r="N5" s="35">
-        <v>2013</v>
-      </c>
-      <c r="O5" s="36">
-        <v>2002</v>
-      </c>
-      <c r="P5" s="34">
-        <v>2003</v>
-      </c>
-      <c r="Q5" s="34">
-        <v>2004</v>
-      </c>
-      <c r="R5" s="34">
-        <v>2005</v>
-      </c>
-      <c r="S5" s="34">
-        <v>2006</v>
-      </c>
-      <c r="T5" s="34">
-        <v>2007</v>
-      </c>
-      <c r="U5" s="34">
-        <v>2008</v>
-      </c>
-      <c r="V5" s="34">
-        <v>2009</v>
-      </c>
-      <c r="W5" s="34">
-        <v>2010</v>
-      </c>
-      <c r="X5" s="34">
-        <v>2011</v>
-      </c>
-      <c r="Y5" s="34">
-        <v>2012</v>
-      </c>
-      <c r="Z5" s="35">
-        <v>2013</v>
-      </c>
-    </row>
-    <row r="6" spans="2:74" ht="16" x14ac:dyDescent="0.2">
-      <c r="B6" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="38">
-        <v>97</v>
-      </c>
-      <c r="D6" s="38">
-        <v>110</v>
-      </c>
-      <c r="E6" s="38">
-        <v>90</v>
-      </c>
-      <c r="F6" s="38">
-        <v>94</v>
-      </c>
-      <c r="G6" s="38">
-        <v>91</v>
-      </c>
-      <c r="H6" s="39">
-        <v>87</v>
-      </c>
-      <c r="I6" s="39">
-        <v>85</v>
-      </c>
-      <c r="J6" s="40">
-        <v>95</v>
-      </c>
-      <c r="K6" s="40">
-        <v>92</v>
-      </c>
-      <c r="L6" s="40">
-        <v>97</v>
-      </c>
-      <c r="M6" s="40">
-        <v>89</v>
-      </c>
-      <c r="N6" s="41">
-        <v>94</v>
-      </c>
-      <c r="O6" s="42">
-        <v>15</v>
-      </c>
-      <c r="P6" s="38">
-        <v>10</v>
-      </c>
-      <c r="Q6" s="38">
-        <v>11</v>
-      </c>
-      <c r="R6" s="38">
-        <v>12</v>
-      </c>
-      <c r="S6" s="38">
-        <v>5</v>
-      </c>
-      <c r="T6" s="38">
-        <v>3</v>
-      </c>
-      <c r="U6" s="38">
-        <v>0</v>
-      </c>
-      <c r="V6" s="43">
-        <v>2</v>
-      </c>
-      <c r="W6" s="43">
-        <v>2</v>
-      </c>
-      <c r="X6" s="43">
-        <v>3</v>
-      </c>
-      <c r="Y6" s="43">
-        <v>3</v>
-      </c>
-      <c r="Z6" s="44">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="2:74" ht="16" x14ac:dyDescent="0.2">
-      <c r="B7" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="38">
-        <v>249</v>
-      </c>
-      <c r="D7" s="38">
-        <v>267</v>
-      </c>
-      <c r="E7" s="38">
-        <v>257</v>
-      </c>
-      <c r="F7" s="38">
-        <v>218</v>
-      </c>
-      <c r="G7" s="38">
-        <v>190</v>
-      </c>
-      <c r="H7" s="39">
-        <v>209</v>
-      </c>
-      <c r="I7" s="39">
-        <v>216</v>
-      </c>
-      <c r="J7" s="40">
-        <v>196</v>
-      </c>
-      <c r="K7" s="40">
-        <v>194</v>
-      </c>
-      <c r="L7" s="40">
-        <v>192</v>
-      </c>
-      <c r="M7" s="40">
-        <v>200</v>
-      </c>
-      <c r="N7" s="41">
-        <v>213</v>
-      </c>
-      <c r="O7" s="42">
-        <v>35</v>
-      </c>
-      <c r="P7" s="38">
-        <v>15</v>
-      </c>
-      <c r="Q7" s="38">
-        <v>7</v>
-      </c>
-      <c r="R7" s="38">
-        <v>43</v>
-      </c>
-      <c r="S7" s="38">
-        <v>66</v>
-      </c>
-      <c r="T7" s="38">
-        <v>74</v>
-      </c>
-      <c r="U7" s="38">
-        <v>42</v>
-      </c>
-      <c r="V7" s="43">
-        <v>43</v>
-      </c>
-      <c r="W7" s="43">
-        <v>45</v>
-      </c>
-      <c r="X7" s="43">
-        <v>33</v>
-      </c>
-      <c r="Y7" s="43">
-        <v>28</v>
-      </c>
-      <c r="Z7" s="44">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="2:74" ht="16" x14ac:dyDescent="0.2">
-      <c r="B8" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="38">
-        <v>54</v>
-      </c>
-      <c r="D8" s="38">
-        <v>62</v>
-      </c>
-      <c r="E8" s="38">
-        <v>56</v>
-      </c>
-      <c r="F8" s="38">
-        <v>67</v>
-      </c>
-      <c r="G8" s="38">
-        <v>75</v>
-      </c>
-      <c r="H8" s="39">
-        <v>82</v>
-      </c>
-      <c r="I8" s="39">
-        <v>79</v>
-      </c>
-      <c r="J8" s="40">
-        <v>70</v>
-      </c>
-      <c r="K8" s="40">
-        <v>68</v>
-      </c>
-      <c r="L8" s="40">
-        <v>69</v>
-      </c>
-      <c r="M8" s="40">
-        <v>58</v>
-      </c>
-      <c r="N8" s="41">
-        <v>64</v>
-      </c>
-      <c r="O8" s="42">
-        <v>50</v>
-      </c>
-      <c r="P8" s="38">
-        <v>16</v>
-      </c>
-      <c r="Q8" s="38">
-        <v>28</v>
-      </c>
-      <c r="R8" s="38">
-        <v>20</v>
-      </c>
-      <c r="S8" s="38">
-        <v>10</v>
-      </c>
-      <c r="T8" s="38">
-        <v>16</v>
-      </c>
-      <c r="U8" s="38">
-        <v>17</v>
-      </c>
-      <c r="V8" s="43">
-        <v>22</v>
-      </c>
-      <c r="W8" s="43">
-        <v>8</v>
-      </c>
-      <c r="X8" s="43">
-        <v>7</v>
-      </c>
-      <c r="Y8" s="43">
-        <v>9</v>
-      </c>
-      <c r="Z8" s="44">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="2:74" ht="16" x14ac:dyDescent="0.2">
-      <c r="B9" s="37" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="38">
-        <v>157</v>
-      </c>
-      <c r="D9" s="38">
-        <v>175</v>
-      </c>
-      <c r="E9" s="38">
-        <v>173</v>
-      </c>
-      <c r="F9" s="38">
-        <v>178</v>
-      </c>
-      <c r="G9" s="38">
-        <v>151</v>
-      </c>
-      <c r="H9" s="39">
-        <v>159</v>
-      </c>
-      <c r="I9" s="39">
-        <v>158</v>
-      </c>
-      <c r="J9" s="40">
-        <v>156</v>
-      </c>
-      <c r="K9" s="40">
-        <v>154</v>
-      </c>
-      <c r="L9" s="40">
-        <v>175</v>
-      </c>
-      <c r="M9" s="40">
-        <v>177</v>
-      </c>
-      <c r="N9" s="41">
-        <v>179</v>
-      </c>
-      <c r="O9" s="42">
-        <v>1</v>
-      </c>
-      <c r="P9" s="38">
-        <v>4</v>
-      </c>
-      <c r="Q9" s="38">
-        <v>4</v>
-      </c>
-      <c r="R9" s="38">
-        <v>0</v>
-      </c>
-      <c r="S9" s="38">
-        <v>6</v>
-      </c>
-      <c r="T9" s="38">
-        <v>6</v>
-      </c>
-      <c r="U9" s="38">
-        <v>12</v>
-      </c>
-      <c r="V9" s="43">
-        <v>2</v>
-      </c>
-      <c r="W9" s="43">
-        <v>10</v>
-      </c>
-      <c r="X9" s="43">
-        <v>9</v>
-      </c>
-      <c r="Y9" s="43">
-        <v>10</v>
-      </c>
-      <c r="Z9" s="44">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="2:74" ht="16" x14ac:dyDescent="0.2">
-      <c r="B10" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="38">
-        <v>370</v>
-      </c>
-      <c r="D10" s="38">
-        <v>402</v>
-      </c>
-      <c r="E10" s="38">
-        <v>394</v>
-      </c>
-      <c r="F10" s="38">
-        <v>381</v>
-      </c>
-      <c r="G10" s="38">
-        <v>394</v>
-      </c>
-      <c r="H10" s="39">
-        <v>417</v>
-      </c>
-      <c r="I10" s="39">
-        <v>408</v>
-      </c>
-      <c r="J10" s="40">
-        <v>425</v>
-      </c>
-      <c r="K10" s="40">
-        <v>356</v>
-      </c>
-      <c r="L10" s="40">
-        <v>303</v>
-      </c>
-      <c r="M10" s="40">
-        <v>291</v>
-      </c>
-      <c r="N10" s="41">
-        <v>295</v>
-      </c>
-      <c r="O10" s="42">
-        <v>31</v>
-      </c>
-      <c r="P10" s="38">
-        <v>29</v>
-      </c>
-      <c r="Q10" s="38">
-        <v>4</v>
-      </c>
-      <c r="R10" s="38">
-        <v>15</v>
-      </c>
-      <c r="S10" s="38">
-        <v>19</v>
-      </c>
-      <c r="T10" s="38">
-        <v>7</v>
-      </c>
-      <c r="U10" s="38">
-        <v>10</v>
-      </c>
-      <c r="V10" s="43">
-        <v>0</v>
-      </c>
-      <c r="W10" s="43">
-        <v>0</v>
-      </c>
-      <c r="X10" s="43">
-        <v>0</v>
-      </c>
-      <c r="Y10" s="43">
-        <v>0</v>
-      </c>
-      <c r="Z10" s="44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:74" ht="16" x14ac:dyDescent="0.2">
-      <c r="B11" s="37" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="38">
-        <v>99</v>
-      </c>
-      <c r="D11" s="38">
-        <v>111</v>
-      </c>
-      <c r="E11" s="38">
-        <v>113</v>
-      </c>
-      <c r="F11" s="38">
-        <v>119</v>
-      </c>
-      <c r="G11" s="38">
-        <v>125</v>
-      </c>
-      <c r="H11" s="39">
-        <v>142</v>
-      </c>
-      <c r="I11" s="39">
-        <v>152</v>
-      </c>
-      <c r="J11" s="40">
-        <v>157</v>
-      </c>
-      <c r="K11" s="40">
-        <v>162</v>
-      </c>
-      <c r="L11" s="40">
-        <v>164</v>
-      </c>
-      <c r="M11" s="40">
-        <v>169</v>
-      </c>
-      <c r="N11" s="41">
-        <v>165</v>
-      </c>
-      <c r="O11" s="42">
-        <v>29</v>
-      </c>
-      <c r="P11" s="38">
-        <v>32</v>
-      </c>
-      <c r="Q11" s="38">
-        <v>23</v>
-      </c>
-      <c r="R11" s="38">
-        <v>35</v>
-      </c>
-      <c r="S11" s="38">
-        <v>27</v>
-      </c>
-      <c r="T11" s="38">
-        <v>26</v>
-      </c>
-      <c r="U11" s="38">
-        <v>16</v>
-      </c>
-      <c r="V11" s="43">
-        <v>8</v>
-      </c>
-      <c r="W11" s="43">
-        <v>4</v>
-      </c>
-      <c r="X11" s="43">
-        <v>4</v>
-      </c>
-      <c r="Y11" s="43">
-        <v>2</v>
-      </c>
-      <c r="Z11" s="44">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="2:74" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="37" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="38">
-        <v>393</v>
-      </c>
-      <c r="D12" s="38">
-        <v>429</v>
-      </c>
-      <c r="E12" s="38">
-        <v>434</v>
-      </c>
-      <c r="F12" s="38">
-        <v>445</v>
-      </c>
-      <c r="G12" s="38">
-        <v>451</v>
-      </c>
-      <c r="H12" s="39">
-        <v>441</v>
-      </c>
-      <c r="I12" s="39">
-        <v>437</v>
-      </c>
-      <c r="J12" s="40">
-        <v>446</v>
-      </c>
-      <c r="K12" s="40">
-        <v>447</v>
-      </c>
-      <c r="L12" s="40">
-        <v>456</v>
-      </c>
-      <c r="M12" s="40">
-        <v>459</v>
-      </c>
-      <c r="N12" s="41">
-        <v>466</v>
-      </c>
-      <c r="O12" s="42">
-        <v>62</v>
-      </c>
-      <c r="P12" s="38">
-        <v>71</v>
-      </c>
-      <c r="Q12" s="38">
-        <v>41</v>
-      </c>
-      <c r="R12" s="38">
-        <v>72</v>
-      </c>
-      <c r="S12" s="38">
-        <v>70</v>
-      </c>
-      <c r="T12" s="38">
-        <v>46</v>
-      </c>
-      <c r="U12" s="38">
-        <v>64</v>
-      </c>
-      <c r="V12" s="43">
-        <v>55</v>
-      </c>
-      <c r="W12" s="43">
-        <v>73</v>
-      </c>
-      <c r="X12" s="43">
-        <v>48</v>
-      </c>
-      <c r="Y12" s="43">
-        <v>25</v>
-      </c>
-      <c r="Z12" s="44">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="2:74" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="46">
-        <v>4522</v>
-      </c>
-      <c r="D13" s="46">
-        <v>4952</v>
-      </c>
-      <c r="E13" s="46">
-        <v>5106</v>
-      </c>
-      <c r="F13" s="46">
-        <v>5177</v>
-      </c>
-      <c r="G13" s="46">
-        <v>5251</v>
-      </c>
-      <c r="H13" s="47">
-        <v>5436</v>
-      </c>
-      <c r="I13" s="47">
-        <v>5500</v>
-      </c>
-      <c r="J13" s="47">
-        <v>5617</v>
-      </c>
-      <c r="K13" s="47">
-        <v>5634</v>
-      </c>
-      <c r="L13" s="47">
-        <v>5595</v>
-      </c>
-      <c r="M13" s="47">
-        <v>5568</v>
-      </c>
-      <c r="N13" s="48">
-        <v>5574</v>
-      </c>
-      <c r="O13" s="49">
-        <v>939</v>
-      </c>
-      <c r="P13" s="46">
-        <v>788</v>
-      </c>
-      <c r="Q13" s="46">
-        <v>601</v>
-      </c>
-      <c r="R13" s="46">
-        <v>589</v>
-      </c>
-      <c r="S13" s="46">
-        <v>629</v>
-      </c>
-      <c r="T13" s="46">
-        <v>594</v>
-      </c>
-      <c r="U13" s="46">
-        <v>524</v>
-      </c>
-      <c r="V13" s="46">
-        <v>422</v>
-      </c>
-      <c r="W13" s="46">
-        <v>444</v>
-      </c>
-      <c r="X13" s="46">
-        <v>327</v>
-      </c>
-      <c r="Y13" s="46">
-        <v>330</v>
-      </c>
-      <c r="Z13" s="50">
-        <v>361</v>
-      </c>
-      <c r="AA13">
-        <v>417</v>
-      </c>
-      <c r="AB13">
-        <v>443</v>
-      </c>
-      <c r="AC13">
-        <v>464</v>
-      </c>
-      <c r="AD13">
-        <v>478</v>
-      </c>
-      <c r="AE13">
-        <v>485</v>
-      </c>
-      <c r="AF13">
-        <v>489</v>
-      </c>
-      <c r="AG13">
-        <v>513</v>
-      </c>
-      <c r="AH13">
-        <v>511</v>
-      </c>
-      <c r="AI13">
-        <v>561</v>
-      </c>
-      <c r="AJ13">
-        <v>563</v>
-      </c>
-      <c r="AK13">
-        <v>580</v>
-      </c>
-      <c r="AL13">
-        <v>584</v>
-      </c>
-      <c r="AM13">
-        <v>162</v>
-      </c>
-      <c r="AN13">
-        <v>293</v>
-      </c>
-      <c r="AO13">
-        <v>486</v>
-      </c>
-      <c r="AP13">
-        <v>696</v>
-      </c>
-      <c r="AQ13">
-        <v>935</v>
-      </c>
-      <c r="AR13" s="1">
-        <v>1143</v>
-      </c>
-      <c r="AS13" s="1">
-        <v>1516</v>
-      </c>
-      <c r="AT13" s="1">
-        <v>2003</v>
-      </c>
-      <c r="AU13" s="1">
-        <v>2380</v>
-      </c>
-      <c r="AV13" s="1">
-        <v>2558</v>
-      </c>
-      <c r="AW13" s="1">
-        <v>2829</v>
-      </c>
-      <c r="AX13" s="1">
-        <v>2717</v>
-      </c>
-      <c r="AY13">
-        <v>249</v>
-      </c>
-      <c r="AZ13">
-        <v>323</v>
-      </c>
-      <c r="BA13">
-        <v>334</v>
-      </c>
-      <c r="BB13">
-        <v>326</v>
-      </c>
-      <c r="BC13">
-        <v>391</v>
-      </c>
-      <c r="BD13">
-        <v>437</v>
-      </c>
-      <c r="BE13">
-        <v>345</v>
-      </c>
-      <c r="BF13">
-        <v>390</v>
-      </c>
-      <c r="BG13">
-        <v>451</v>
-      </c>
-      <c r="BH13">
-        <v>492</v>
-      </c>
-      <c r="BI13">
-        <v>604</v>
-      </c>
-      <c r="BJ13">
-        <v>663</v>
-      </c>
-      <c r="BK13" s="1">
-        <v>6289</v>
-      </c>
-      <c r="BL13" s="1">
-        <v>6799</v>
-      </c>
-      <c r="BM13" s="1">
-        <v>6991</v>
-      </c>
-      <c r="BN13" s="1">
-        <v>7266</v>
-      </c>
-      <c r="BO13" s="1">
-        <v>7691</v>
-      </c>
-      <c r="BP13" s="1">
-        <v>8099</v>
-      </c>
-      <c r="BQ13" s="1">
-        <v>8398</v>
-      </c>
-      <c r="BR13" s="1">
-        <v>8943</v>
-      </c>
-      <c r="BS13" s="1">
-        <v>9470</v>
-      </c>
-      <c r="BT13" s="1">
-        <v>9535</v>
-      </c>
-      <c r="BU13" s="1">
-        <v>9911</v>
-      </c>
-      <c r="BV13" s="1">
-        <v>9899</v>
-      </c>
-    </row>
-    <row r="14" spans="2:74" ht="16" x14ac:dyDescent="0.2">
-      <c r="B14" s="51"/>
-      <c r="C14" s="51"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="51"/>
-      <c r="H14" s="52"/>
-      <c r="I14" s="52"/>
-      <c r="J14" s="52"/>
-      <c r="K14" s="52"/>
-      <c r="L14" s="52"/>
-      <c r="M14" s="52"/>
-      <c r="N14" s="52"/>
-      <c r="O14" s="51"/>
-      <c r="P14" s="51"/>
-      <c r="Q14" s="51"/>
-      <c r="R14" s="51"/>
-      <c r="S14" s="51"/>
-      <c r="T14" s="51"/>
-      <c r="U14" s="51"/>
-      <c r="V14" s="51"/>
-      <c r="W14" s="51"/>
-      <c r="X14" s="51"/>
-      <c r="Y14" s="51"/>
-      <c r="Z14" s="51"/>
-    </row>
-    <row r="15" spans="2:74" ht="16" x14ac:dyDescent="0.2">
-      <c r="B15" s="51" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="51"/>
-      <c r="D15" s="51"/>
-      <c r="E15" s="51"/>
-      <c r="F15" s="51"/>
-      <c r="G15" s="51"/>
-      <c r="H15" s="52"/>
-      <c r="I15" s="52"/>
-      <c r="J15" s="52"/>
-      <c r="K15" s="52"/>
-      <c r="L15" s="52"/>
-      <c r="M15" s="52"/>
-      <c r="N15" s="52"/>
-      <c r="O15" s="51"/>
-      <c r="P15" s="51"/>
-      <c r="Q15" s="51"/>
-      <c r="R15" s="51"/>
-      <c r="S15" s="51"/>
-      <c r="T15" s="51"/>
-      <c r="U15" s="51"/>
-      <c r="V15" s="51"/>
-      <c r="W15" s="51"/>
-      <c r="X15" s="51"/>
-      <c r="Y15" s="51"/>
-      <c r="Z15" s="51"/>
-    </row>
-    <row r="16" spans="2:74" ht="16" x14ac:dyDescent="0.2">
-      <c r="B16" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="51"/>
-      <c r="D16" s="51"/>
-      <c r="E16" s="51"/>
-      <c r="F16" s="51"/>
-      <c r="G16" s="51"/>
-      <c r="H16" s="52"/>
-      <c r="I16" s="52"/>
-      <c r="J16" s="52"/>
-      <c r="K16" s="52"/>
-      <c r="L16" s="52"/>
-      <c r="M16" s="52"/>
-      <c r="N16" s="52"/>
-      <c r="O16" s="51"/>
-      <c r="P16" s="51"/>
-      <c r="Q16" s="51"/>
-      <c r="R16" s="51"/>
-      <c r="S16" s="51"/>
-      <c r="T16" s="51"/>
-      <c r="U16" s="51"/>
-      <c r="V16" s="51"/>
-      <c r="W16" s="51"/>
-      <c r="X16" s="51"/>
-      <c r="Y16" s="51"/>
-      <c r="Z16" s="51"/>
-    </row>
-    <row r="17" spans="2:26" ht="16" x14ac:dyDescent="0.2">
-      <c r="B17" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="51"/>
-      <c r="D17" s="51"/>
-      <c r="E17" s="51"/>
-      <c r="F17" s="51"/>
-      <c r="G17" s="51"/>
-      <c r="H17" s="52"/>
-      <c r="I17" s="52"/>
-      <c r="J17" s="52"/>
-      <c r="K17" s="52"/>
-      <c r="L17" s="52"/>
-      <c r="M17" s="52"/>
-      <c r="N17" s="52"/>
-      <c r="O17" s="51"/>
-      <c r="P17" s="51"/>
-      <c r="Q17" s="51"/>
-      <c r="R17" s="51"/>
-      <c r="S17" s="51"/>
-      <c r="T17" s="51"/>
-      <c r="U17" s="51"/>
-      <c r="V17" s="51"/>
-      <c r="W17" s="51"/>
-      <c r="X17" s="51"/>
-      <c r="Y17" s="51"/>
-      <c r="Z17" s="51"/>
-    </row>
-    <row r="18" spans="2:26" ht="16" x14ac:dyDescent="0.2">
-      <c r="B18" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="51"/>
-      <c r="D18" s="51"/>
-      <c r="E18" s="51"/>
-      <c r="F18" s="51"/>
-      <c r="G18" s="51"/>
-      <c r="H18" s="52"/>
-      <c r="I18" s="52"/>
-      <c r="J18" s="52"/>
-      <c r="K18" s="52"/>
-      <c r="L18" s="52"/>
-      <c r="M18" s="52"/>
-      <c r="N18" s="52"/>
-      <c r="O18" s="51"/>
-      <c r="P18" s="51"/>
-      <c r="Q18" s="51"/>
-      <c r="R18" s="51"/>
-      <c r="S18" s="51"/>
-      <c r="T18" s="51"/>
-      <c r="U18" s="51"/>
-      <c r="V18" s="51"/>
-      <c r="W18" s="51"/>
-      <c r="X18" s="51"/>
-      <c r="Y18" s="51"/>
-      <c r="Z18" s="51"/>
-    </row>
-    <row r="19" spans="2:26" ht="16" x14ac:dyDescent="0.2">
-      <c r="B19" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="53"/>
-      <c r="D19" s="53"/>
-      <c r="E19" s="53"/>
-      <c r="F19" s="53"/>
-      <c r="G19" s="53"/>
-      <c r="H19" s="39"/>
-      <c r="I19" s="39"/>
-      <c r="J19" s="39"/>
-      <c r="K19" s="39"/>
-      <c r="L19" s="39"/>
-      <c r="M19" s="39"/>
-      <c r="N19" s="39"/>
-      <c r="O19" s="53"/>
-      <c r="P19" s="53"/>
-      <c r="Q19" s="53"/>
-      <c r="R19" s="53"/>
-      <c r="S19" s="53"/>
-      <c r="T19" s="53"/>
-      <c r="U19" s="53"/>
-      <c r="V19" s="53"/>
-      <c r="W19" s="53"/>
-      <c r="X19" s="53"/>
-      <c r="Y19" s="53"/>
-      <c r="Z19" s="53"/>
-    </row>
-    <row r="20" spans="2:26" ht="16" x14ac:dyDescent="0.2">
-      <c r="B20" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" s="53"/>
-      <c r="D20" s="53"/>
-      <c r="E20" s="53"/>
-      <c r="F20" s="53"/>
-      <c r="G20" s="53"/>
-      <c r="H20" s="39"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
-      <c r="K20" s="39"/>
-      <c r="L20" s="39"/>
-      <c r="M20" s="39"/>
-      <c r="N20" s="39"/>
-      <c r="O20" s="53"/>
-      <c r="P20" s="53"/>
-      <c r="Q20" s="53"/>
-      <c r="R20" s="53"/>
-      <c r="S20" s="53"/>
-      <c r="T20" s="53"/>
-      <c r="U20" s="53"/>
-      <c r="V20" s="53"/>
-      <c r="W20" s="53"/>
-      <c r="X20" s="53"/>
-      <c r="Y20" s="53"/>
-      <c r="Z20" s="53"/>
-    </row>
-    <row r="21" spans="2:26" ht="16" x14ac:dyDescent="0.2">
-      <c r="B21" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="53"/>
-      <c r="D21" s="53"/>
-      <c r="E21" s="53"/>
-      <c r="F21" s="53"/>
-      <c r="G21" s="53"/>
-      <c r="H21" s="39"/>
-      <c r="I21" s="39"/>
-      <c r="J21" s="39"/>
-      <c r="K21" s="39"/>
-      <c r="L21" s="39"/>
-      <c r="M21" s="39"/>
-      <c r="N21" s="39"/>
-      <c r="O21" s="53"/>
-      <c r="P21" s="53"/>
-      <c r="Q21" s="53"/>
-      <c r="R21" s="53"/>
-      <c r="S21" s="53"/>
-      <c r="T21" s="53"/>
-      <c r="U21" s="53"/>
-      <c r="V21" s="53"/>
-      <c r="W21" s="53"/>
-      <c r="X21" s="53"/>
-      <c r="Y21" s="53"/>
-      <c r="Z21" s="53"/>
-    </row>
-    <row r="22" spans="2:26" ht="16" x14ac:dyDescent="0.2">
-      <c r="B22" s="38" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="53"/>
-      <c r="D22" s="53"/>
-      <c r="E22" s="53"/>
-      <c r="F22" s="53"/>
-      <c r="G22" s="53"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="39"/>
-      <c r="J22" s="39"/>
-      <c r="K22" s="39"/>
-      <c r="L22" s="39"/>
-      <c r="M22" s="39"/>
-      <c r="N22" s="39"/>
-      <c r="O22" s="53"/>
-      <c r="P22" s="53"/>
-      <c r="Q22" s="53"/>
-      <c r="R22" s="53"/>
-      <c r="S22" s="53"/>
-      <c r="T22" s="53"/>
-      <c r="U22" s="53"/>
-      <c r="V22" s="53"/>
-      <c r="W22" s="53"/>
-      <c r="X22" s="53"/>
-      <c r="Y22" s="53"/>
-      <c r="Z22" s="53"/>
-    </row>
-    <row r="23" spans="2:26" ht="16" x14ac:dyDescent="0.2">
-      <c r="B23" s="38" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" s="53"/>
-      <c r="D23" s="53"/>
-      <c r="E23" s="53"/>
-      <c r="F23" s="53"/>
-      <c r="G23" s="53"/>
-      <c r="H23" s="39"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="39"/>
-      <c r="K23" s="39"/>
-      <c r="L23" s="39"/>
-      <c r="M23" s="39"/>
-      <c r="N23" s="39"/>
-      <c r="O23" s="53"/>
-      <c r="P23" s="53"/>
-      <c r="Q23" s="53"/>
-      <c r="R23" s="53"/>
-      <c r="S23" s="53"/>
-      <c r="T23" s="53"/>
-      <c r="U23" s="53"/>
-      <c r="V23" s="53"/>
-      <c r="W23" s="53"/>
-      <c r="X23" s="53"/>
-      <c r="Y23" s="53"/>
-      <c r="Z23" s="53"/>
-    </row>
-    <row r="24" spans="2:26" ht="16" x14ac:dyDescent="0.2">
-      <c r="B24" s="51" t="s">
-        <v>38</v>
-      </c>
-      <c r="C24" s="53"/>
-      <c r="D24" s="53"/>
-      <c r="E24" s="53"/>
-      <c r="F24" s="53"/>
-      <c r="G24" s="53"/>
-      <c r="H24" s="53"/>
-      <c r="I24" s="53"/>
-      <c r="J24" s="53"/>
-      <c r="K24" s="53"/>
-      <c r="L24" s="53"/>
-      <c r="M24" s="53"/>
-      <c r="N24" s="53"/>
-      <c r="O24" s="53"/>
-      <c r="P24" s="53"/>
-      <c r="Q24" s="53"/>
-      <c r="R24" s="53"/>
-      <c r="S24" s="53"/>
-      <c r="T24" s="53"/>
-      <c r="U24" s="53"/>
-      <c r="V24" s="53"/>
-      <c r="W24" s="53"/>
-      <c r="X24" s="53"/>
-      <c r="Y24" s="53"/>
-      <c r="Z24" s="53"/>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="C3:Z3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:N4"/>
-    <mergeCell ref="O4:Z4"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>